<commit_message>
inizio lavoro su parametri PMos
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CONTROLLO VERSIONE\MICROA\MicroB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101A3DFE-17D9-49FF-9F25-488DA32F30DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CD5233-7A6E-41F1-930A-1F050EB46ADE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="2115" windowWidth="24150" windowHeight="13035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Ib</t>
   </si>
@@ -111,17 +112,59 @@
     <t>Vgs</t>
   </si>
   <si>
-    <t>W/L=1</t>
-  </si>
-  <si>
-    <t>Id</t>
+    <t>Vds1</t>
+  </si>
+  <si>
+    <t>Vds2</t>
+  </si>
+  <si>
+    <t>Ids1</t>
+  </si>
+  <si>
+    <t>Ids2</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Va </t>
+  </si>
+  <si>
+    <t>1/lambda</t>
+  </si>
+  <si>
+    <t>(dI/dV)/Ids_sat</t>
+  </si>
+  <si>
+    <t>1/R0</t>
+  </si>
+  <si>
+    <t>dI/dV</t>
+  </si>
+  <si>
+    <t>R0</t>
+  </si>
+  <si>
+    <t>NMOS</t>
+  </si>
+  <si>
+    <t>Ids_sat</t>
+  </si>
+  <si>
+    <t>Va_fornito</t>
+  </si>
+  <si>
+    <t>R0_con_Va_fornito</t>
+  </si>
+  <si>
+    <t>gm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,13 +180,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -158,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -167,6 +232,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -483,15 +553,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
     <col min="14" max="14" width="21.140625" customWidth="1"/>
     <col min="16" max="16" width="28.85546875" customWidth="1"/>
   </cols>
@@ -720,113 +790,6 @@
         <v>6.586000000000001E-5</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>-1.4520776403514901E-7</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>0.30000001192092896</v>
-      </c>
-      <c r="C44">
-        <v>-1.588607645430784E-8</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>0.60000002384185791</v>
-      </c>
-      <c r="C45">
-        <v>6.6201874915350345E-7</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <v>0.89999997615814209</v>
-      </c>
-      <c r="C46">
-        <v>8.7598918980802409E-6</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>1.2000000476837158</v>
-      </c>
-      <c r="C47">
-        <v>2.5520826966385357E-5</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>1.5</v>
-      </c>
-      <c r="C48">
-        <v>4.9716374633135274E-5</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>1.7999999523162842</v>
-      </c>
-      <c r="C49">
-        <v>8.0221696407534182E-5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>2.0999999046325684</v>
-      </c>
-      <c r="C50">
-        <v>1.1597821867326275E-4</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>2.4000000953674316</v>
-      </c>
-      <c r="C51">
-        <v>1.5604191867168993E-4</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>2.7000000476837158</v>
-      </c>
-      <c r="C52">
-        <v>1.9960060308221728E-4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <v>3</v>
-      </c>
-      <c r="C53">
-        <v>2.4597617448307574E-4</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54">
-        <v>3.2999999523162842</v>
-      </c>
-      <c r="C54">
-        <v>2.94617930194363E-4</v>
-      </c>
-    </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
     </row>
@@ -1190,6 +1153,1919 @@
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E533CDB7-452E-4AEE-B021-5A11B297142C}">
+  <dimension ref="C3:Z39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="G3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+    </row>
+    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="10">
+        <f>D6-0.4</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="F6" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G6" s="10">
+        <v>9.1685244285599765E-8</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1.08744465876498E-7</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="10">
+        <f>((H6-G6)/(F6-E6))/G6</f>
+        <v>5.8144653359373723E-2</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="10">
+        <f>1/J6</f>
+        <v>17.19848588346234</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="10">
+        <f>((H6-G6)/(F6-E6))</f>
+        <v>5.3310067471556985E-9</v>
+      </c>
+      <c r="O6" s="8"/>
+      <c r="P6" s="10">
+        <f>1/N6</f>
+        <v>187581829.74229759</v>
+      </c>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="10">
+        <v>125</v>
+      </c>
+      <c r="S6" s="8"/>
+      <c r="T6" s="10">
+        <f>$R$6/G6</f>
+        <v>1363360058.3603692</v>
+      </c>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="10">
+        <v>5.000000074505806E-2</v>
+      </c>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="10">
+        <v>8.7849491592351114E-7</v>
+      </c>
+      <c r="Z6" s="8"/>
+    </row>
+    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+      <c r="D7" s="10">
+        <f>D6+0.1</f>
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" ref="E7:E34" si="0">D7-0.4</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="F7" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G7" s="10">
+        <v>6.6201874915350345E-7</v>
+      </c>
+      <c r="H7" s="10">
+        <v>7.3098397024295991E-7</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="10">
+        <f t="shared" ref="J7:J34" si="1">((H7-G7)/(F7-E7))/G7</f>
+        <v>3.3604555069133665E-2</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="10">
+        <f t="shared" ref="L7:L34" si="2">1/J7</f>
+        <v>29.757870560783481</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="10">
+        <f t="shared" ref="N7:N34" si="3">((H7-G7)/(F7-E7))</f>
+        <v>2.2246845512727894E-8</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="10">
+        <f t="shared" ref="P7:P34" si="4">1/N7</f>
+        <v>44950193.025248401</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="10">
+        <f t="shared" ref="T7:T34" si="5">$R$6/G7</f>
+        <v>188816404.61064348</v>
+      </c>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="10">
+        <v>0.15000000596046448</v>
+      </c>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="10">
+        <v>2.5825960392467096E-7</v>
+      </c>
+      <c r="Z7" s="8"/>
+    </row>
+    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+      <c r="D8" s="10">
+        <f>D7+0.1</f>
+        <v>0.7</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="F8" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2.2830251964478521E-6</v>
+      </c>
+      <c r="H8" s="10">
+        <v>2.4430669327557553E-6</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="10">
+        <f t="shared" si="1"/>
+        <v>2.3366910500580745E-2</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="10">
+        <f t="shared" si="2"/>
+        <v>42.795559129442751</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="10">
+        <f t="shared" si="3"/>
+        <v>5.3347245435967729E-8</v>
+      </c>
+      <c r="O8" s="8"/>
+      <c r="P8" s="10">
+        <f t="shared" si="4"/>
+        <v>18745110.301904753</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="10">
+        <f t="shared" si="5"/>
+        <v>54751914.343515307</v>
+      </c>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="10">
+        <v>1.5646232043309283E-7</v>
+      </c>
+      <c r="Z8" s="8"/>
+    </row>
+    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="D9" s="10">
+        <f>D8+0.1</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="F9" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G9" s="10">
+        <v>5.0172225201094989E-6</v>
+      </c>
+      <c r="H9" s="10">
+        <v>5.2841910473944154E-6</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="10">
+        <f t="shared" si="1"/>
+        <v>1.8348421360202819E-2</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="10">
+        <f t="shared" si="2"/>
+        <v>54.500601461495229</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="10">
+        <f t="shared" si="3"/>
+        <v>9.2058112856867753E-8</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="10">
+        <f t="shared" si="4"/>
+        <v>10862703.665833376</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="10">
+        <f t="shared" si="5"/>
+        <v>24914182.996466324</v>
+      </c>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="10">
+        <v>0.35000002384185791</v>
+      </c>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="10">
+        <v>1.5886077164850576E-7</v>
+      </c>
+      <c r="Z9" s="8"/>
+    </row>
+    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C10" s="8"/>
+      <c r="D10" s="10">
+        <f>D9+0.1</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="0"/>
+        <v>0.49999999999999989</v>
+      </c>
+      <c r="F10" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G10" s="10">
+        <v>8.7598918980802409E-6</v>
+      </c>
+      <c r="H10" s="10">
+        <v>9.1380434241727926E-6</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5417326838385204E-2</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="10">
+        <f t="shared" si="2"/>
+        <v>64.862087343848458</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="10">
+        <f t="shared" si="3"/>
+        <v>1.3505411646162561E-7</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="10">
+        <f t="shared" si="4"/>
+        <v>7404439.2440577019</v>
+      </c>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="10">
+        <f t="shared" si="5"/>
+        <v>14269582.485075433</v>
+      </c>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="10">
+        <v>0.44999998807907104</v>
+      </c>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="10">
+        <v>9.1685251391027123E-7</v>
+      </c>
+      <c r="Z10" s="8"/>
+    </row>
+    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C11" s="8"/>
+      <c r="D11" s="10">
+        <f>D10+0.1</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="0"/>
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1.3451834092848003E-5</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1.394151240674546E-5</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="10">
+        <f t="shared" si="1"/>
+        <v>1.3482350230364894E-2</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="10">
+        <f t="shared" si="2"/>
+        <v>74.171044581515474</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="10">
+        <f t="shared" si="3"/>
+        <v>1.8136233848053962E-7</v>
+      </c>
+      <c r="O11" s="8"/>
+      <c r="P11" s="10">
+        <f t="shared" si="4"/>
+        <v>5513823.9194423547</v>
+      </c>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="10">
+        <f t="shared" si="5"/>
+        <v>9292413.1488106381</v>
+      </c>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="10">
+        <v>0.55000001192092896</v>
+      </c>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="10">
+        <v>5.7033334996958729E-6</v>
+      </c>
+      <c r="Z11" s="8"/>
+    </row>
+    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C12" s="8"/>
+      <c r="D12" s="10">
+        <f>D11+0.1</f>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.69999999999999984</v>
+      </c>
+      <c r="F12" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1.9052218704018742E-5</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1.9651763068395667E-5</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="10">
+        <f t="shared" si="1"/>
+        <v>1.2103261561351769E-2</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="10">
+        <f t="shared" si="2"/>
+        <v>82.622357199418701</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="10">
+        <f t="shared" si="3"/>
+        <v>2.3059398629881727E-7</v>
+      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="10">
+        <f t="shared" si="4"/>
+        <v>4336626.5358895399</v>
+      </c>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="10">
+        <f t="shared" si="5"/>
+        <v>6560915.6572212437</v>
+      </c>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="10">
+        <v>0.64999997615814209</v>
+      </c>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="10">
+        <v>1.6210071407840587E-5</v>
+      </c>
+      <c r="Z12" s="8"/>
+    </row>
+    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C13" s="8"/>
+      <c r="D13" s="10">
+        <f>D12+0.1</f>
+        <v>1.2</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="F13" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G13" s="10">
+        <v>2.5520826966385357E-5</v>
+      </c>
+      <c r="H13" s="10">
+        <v>2.6227080525131896E-5</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="10">
+        <f t="shared" si="1"/>
+        <v>1.1069446294616984E-2</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="10">
+        <f t="shared" si="2"/>
+        <v>90.338755289530155</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="10">
+        <f t="shared" si="3"/>
+        <v>2.825014234986156E-7</v>
+      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="10">
+        <f t="shared" si="4"/>
+        <v>3539805.1720079225</v>
+      </c>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="10">
+        <f t="shared" si="5"/>
+        <v>4897960.4056186415</v>
+      </c>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="10">
+        <v>2.7341966415406205E-5</v>
+      </c>
+      <c r="Z13" s="8"/>
+    </row>
+    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C14" s="8"/>
+      <c r="D14" s="10">
+        <f>D13+0.1</f>
+        <v>1.3</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="F14" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G14" s="10">
+        <v>3.2815929444041103E-5</v>
+      </c>
+      <c r="H14" s="10">
+        <v>3.3624524803599343E-5</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="10">
+        <f t="shared" si="1"/>
+        <v>1.0266804532347181E-2</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="10">
+        <f t="shared" si="2"/>
+        <v>97.401289451780528</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="10">
+        <f t="shared" si="3"/>
+        <v>3.3691473314926651E-7</v>
+      </c>
+      <c r="O14" s="8"/>
+      <c r="P14" s="10">
+        <f t="shared" si="4"/>
+        <v>2968110.0338136908</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="10">
+        <f t="shared" si="5"/>
+        <v>3809125.6934579429</v>
+      </c>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="10">
+        <v>0.85000002384185791</v>
+      </c>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="10">
+        <v>3.7426707422127947E-5</v>
+      </c>
+      <c r="Z14" s="8"/>
+    </row>
+    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C15" s="8"/>
+      <c r="D15" s="10">
+        <f>D14+0.1</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G15" s="10">
+        <v>4.0895170968724415E-5</v>
+      </c>
+      <c r="H15" s="10">
+        <v>4.1800743929343298E-5</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="10">
+        <f t="shared" si="1"/>
+        <v>9.6277229035974903E-3</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="10">
+        <f t="shared" si="2"/>
+        <v>103.86672009705852</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="10">
+        <f t="shared" si="3"/>
+        <v>3.9372737418212322E-7</v>
+      </c>
+      <c r="O15" s="8"/>
+      <c r="P15" s="10">
+        <f t="shared" si="4"/>
+        <v>2539828.4843091411</v>
+      </c>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="10">
+        <f t="shared" si="5"/>
+        <v>3056595.6086990521</v>
+      </c>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="10">
+        <v>0.94999998807907104</v>
+      </c>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="10">
+        <v>4.6919409214751795E-5</v>
+      </c>
+      <c r="Z15" s="8"/>
+    </row>
+    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C16" s="8"/>
+      <c r="D16" s="10">
+        <f>D15+0.1</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F16" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G16" s="10">
+        <v>4.9716374633135274E-5</v>
+      </c>
+      <c r="H16" s="10">
+        <v>5.0712751544779167E-5</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="10">
+        <f t="shared" si="1"/>
+        <v>9.1096464604222913E-3</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="10">
+        <f t="shared" si="2"/>
+        <v>109.77374416719609</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="10">
+        <f t="shared" si="3"/>
+        <v>4.5289859620176936E-7</v>
+      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="10">
+        <f t="shared" si="4"/>
+        <v>2207999.7782869996</v>
+      </c>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="10">
+        <f t="shared" si="5"/>
+        <v>2514262.1706106709</v>
+      </c>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="10">
+        <v>1.0499999523162842</v>
+      </c>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="10">
+        <v>5.6003831559792161E-5</v>
+      </c>
+      <c r="Z16" s="8"/>
+    </row>
+    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C17" s="8"/>
+      <c r="D17" s="10">
+        <f>D16+0.1</f>
+        <v>1.6000000000000003</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="F17" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G17" s="10">
+        <v>5.9238034737063572E-5</v>
+      </c>
+      <c r="H17" s="10">
+        <v>6.0318350733723491E-5</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="10">
+        <f t="shared" si="1"/>
+        <v>8.6842210611657554E-3</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="10">
+        <f t="shared" si="2"/>
+        <v>115.15137546092841</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="10">
+        <f t="shared" si="3"/>
+        <v>5.1443618888567605E-7</v>
+      </c>
+      <c r="O17" s="8"/>
+      <c r="P17" s="10">
+        <f t="shared" si="4"/>
+        <v>1943875.6868293174</v>
+      </c>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="10">
+        <f t="shared" si="5"/>
+        <v>2110130.7724814005</v>
+      </c>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="10">
+        <v>1.1500000953674316</v>
+      </c>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="10">
+        <v>6.4686064433772117E-5</v>
+      </c>
+      <c r="Z17" s="8"/>
+    </row>
+    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C18" s="8"/>
+      <c r="D18" s="10">
+        <f>D17+0.1</f>
+        <v>1.7000000000000004</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="0"/>
+        <v>1.3000000000000003</v>
+      </c>
+      <c r="F18" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G18" s="10">
+        <v>6.9419598730746657E-5</v>
+      </c>
+      <c r="H18" s="10">
+        <v>7.0576395955868065E-5</v>
+      </c>
+      <c r="I18" s="8"/>
+      <c r="J18" s="10">
+        <f t="shared" si="1"/>
+        <v>8.331921001216127E-3</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="10">
+        <f t="shared" si="2"/>
+        <v>120.02034102988254</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="10">
+        <f t="shared" si="3"/>
+        <v>5.7839861256070446E-7</v>
+      </c>
+      <c r="O18" s="8"/>
+      <c r="P18" s="10">
+        <f t="shared" si="4"/>
+        <v>1728911.4778003506</v>
+      </c>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="10">
+        <f t="shared" si="5"/>
+        <v>1800644.2313910439</v>
+      </c>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="10">
+        <v>7.2951093898154795E-5</v>
+      </c>
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C19" s="8"/>
+      <c r="D19" s="10">
+        <f>D18+0.1</f>
+        <v>1.8000000000000005</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000004</v>
+      </c>
+      <c r="F19" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G19" s="10">
+        <v>8.0221696407534182E-5</v>
+      </c>
+      <c r="H19" s="10">
+        <v>8.1447004049550742E-5</v>
+      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="10">
+        <f t="shared" si="1"/>
+        <v>8.0389568886693012E-3</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19" s="10">
+        <f t="shared" si="2"/>
+        <v>124.39424838929958</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="10">
+        <f t="shared" si="3"/>
+        <v>6.4489875895608432E-7</v>
+      </c>
+      <c r="O19" s="8"/>
+      <c r="P19" s="10">
+        <f t="shared" si="4"/>
+        <v>1550630.9883720789</v>
+      </c>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="10">
+        <f t="shared" si="5"/>
+        <v>1558181.9582197263</v>
+      </c>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="10">
+        <v>1.3499999046325684</v>
+      </c>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="10">
+        <v>8.0792393418960273E-5</v>
+      </c>
+      <c r="Z19" s="8"/>
+    </row>
+    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C20" s="8"/>
+      <c r="D20" s="10">
+        <f>D19+0.1</f>
+        <v>1.9000000000000006</v>
+      </c>
+      <c r="E20" s="10">
+        <f t="shared" si="0"/>
+        <v>1.5000000000000004</v>
+      </c>
+      <c r="F20" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G20" s="10">
+        <v>9.160628542304039E-5</v>
+      </c>
+      <c r="H20" s="10">
+        <v>9.2891641543246806E-5</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="10">
+        <f t="shared" si="1"/>
+        <v>7.7951718067197735E-3</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="10">
+        <f t="shared" si="2"/>
+        <v>128.28453622253161</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="10">
+        <f t="shared" si="3"/>
+        <v>7.1408673344800898E-7</v>
+      </c>
+      <c r="O20" s="8"/>
+      <c r="P20" s="10">
+        <f t="shared" si="4"/>
+        <v>1400390.1111163939</v>
+      </c>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="10">
+        <f t="shared" si="5"/>
+        <v>1364535.1890729605</v>
+      </c>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="10">
+        <v>1.4500000476837158</v>
+      </c>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="10">
+        <v>8.8212014816235751E-5</v>
+      </c>
+      <c r="Z20" s="8"/>
+    </row>
+    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C21" s="8"/>
+      <c r="D21" s="10">
+        <f>D20+0.1</f>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="E21" s="10">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000005</v>
+      </c>
+      <c r="F21" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G21" s="10">
+        <v>1.0353680409025401E-4</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1.0487325926078483E-4</v>
+      </c>
+      <c r="I21" s="8"/>
+      <c r="J21" s="10">
+        <f t="shared" si="1"/>
+        <v>7.5929531263777116E-3</v>
+      </c>
+      <c r="K21" s="8"/>
+      <c r="L21" s="10">
+        <f t="shared" si="2"/>
+        <v>131.70106325640643</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="N21" s="10">
+        <f t="shared" si="3"/>
+        <v>7.8615010031225078E-7</v>
+      </c>
+      <c r="O21" s="8"/>
+      <c r="P21" s="10">
+        <f t="shared" si="4"/>
+        <v>1272021.7164671356</v>
+      </c>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="10">
+        <f t="shared" si="5"/>
+        <v>1207300.1586086848</v>
+      </c>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="10">
+        <v>1.5499999523162842</v>
+      </c>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="10">
+        <v>9.5216579211410135E-5</v>
+      </c>
+      <c r="Z21" s="8"/>
+    </row>
+    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C22" s="8"/>
+      <c r="D22" s="10">
+        <f>D21+0.1</f>
+        <v>2.1000000000000005</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" si="0"/>
+        <v>1.7000000000000006</v>
+      </c>
+      <c r="F22" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G22" s="10">
+        <v>1.1597821867326275E-4</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1.1735635052900761E-4</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="10">
+        <f t="shared" si="1"/>
+        <v>7.4266739021670468E-3</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="10">
+        <f t="shared" si="2"/>
+        <v>134.6497790495699</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="N22" s="10">
+        <f t="shared" si="3"/>
+        <v>8.6133240984054325E-7</v>
+      </c>
+      <c r="O22" s="8"/>
+      <c r="P22" s="10">
+        <f t="shared" si="4"/>
+        <v>1160991.9568510465</v>
+      </c>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="10">
+        <f t="shared" si="5"/>
+        <v>1077788.5833214398</v>
+      </c>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="10">
+        <v>1.6500000953674316</v>
+      </c>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="10">
+        <v>1.0181561810895801E-4</v>
+      </c>
+      <c r="Z22" s="8"/>
+    </row>
+    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C23" s="8"/>
+      <c r="D23" s="10">
+        <f>D22+0.1</f>
+        <v>2.2000000000000006</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="F23" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G23" s="10">
+        <v>1.2889709614682943E-4</v>
+      </c>
+      <c r="H23" s="10">
+        <v>1.3030700210947543E-4</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="10">
+        <f t="shared" si="1"/>
+        <v>7.2921527057519557E-3</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" s="10">
+        <f t="shared" si="2"/>
+        <v>137.13371624969028</v>
+      </c>
+      <c r="M23" s="8"/>
+      <c r="N23" s="10">
+        <f t="shared" si="3"/>
+        <v>9.3993730843067222E-7</v>
+      </c>
+      <c r="O23" s="8"/>
+      <c r="P23" s="10">
+        <f t="shared" si="4"/>
+        <v>1063900.7421352484</v>
+      </c>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="10">
+        <f t="shared" si="5"/>
+        <v>969765.8344266332</v>
+      </c>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="10">
+        <v>1.75</v>
+      </c>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="10">
+        <v>1.0802107863128185E-4</v>
+      </c>
+      <c r="Z23" s="8"/>
+    </row>
+    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C24" s="8"/>
+      <c r="D24" s="10">
+        <f>D23+0.1</f>
+        <v>2.3000000000000007</v>
+      </c>
+      <c r="E24" s="10">
+        <f t="shared" si="0"/>
+        <v>1.9000000000000008</v>
+      </c>
+      <c r="F24" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G24" s="10">
+        <v>1.422617060597986E-4</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1.4369290147442371E-4</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="10">
+        <f t="shared" si="1"/>
+        <v>7.1859284366252909E-3</v>
+      </c>
+      <c r="K24" s="8"/>
+      <c r="L24" s="10">
+        <f t="shared" si="2"/>
+        <v>139.16086262468087</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0222824390179352E-6</v>
+      </c>
+      <c r="O24" s="8"/>
+      <c r="P24" s="10">
+        <f t="shared" si="4"/>
+        <v>978203.24582769803</v>
+      </c>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="10">
+        <f t="shared" si="5"/>
+        <v>878662.31512405188</v>
+      </c>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="10">
+        <v>1.8499999046325684</v>
+      </c>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="10">
+        <v>1.1384586105123162E-4</v>
+      </c>
+      <c r="Z24" s="8"/>
+    </row>
+    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C25" s="8"/>
+      <c r="D25" s="10">
+        <f>D24+0.1</f>
+        <v>2.4000000000000008</v>
+      </c>
+      <c r="E25" s="10">
+        <f t="shared" si="0"/>
+        <v>2.0000000000000009</v>
+      </c>
+      <c r="F25" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G25" s="10">
+        <v>1.5604191867168993E-4</v>
+      </c>
+      <c r="H25" s="10">
+        <v>1.5748334408272058E-4</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="10">
+        <f t="shared" si="1"/>
+        <v>7.1057109983937213E-3</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="10">
+        <f t="shared" si="2"/>
+        <v>140.73187049488146</v>
+      </c>
+      <c r="M25" s="8"/>
+      <c r="N25" s="10">
+        <f t="shared" si="3"/>
+        <v>1.1087887777158857E-6</v>
+      </c>
+      <c r="O25" s="8"/>
+      <c r="P25" s="10">
+        <f t="shared" si="4"/>
+        <v>901885.02995133889</v>
+      </c>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="10">
+        <f t="shared" si="5"/>
+        <v>801066.79707648489</v>
+      </c>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="10">
+        <v>1.9500000476837158</v>
+      </c>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="10">
+        <v>1.1930515756830573E-4</v>
+      </c>
+      <c r="Z25" s="8"/>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C26" s="8"/>
+      <c r="D26" s="10">
+        <f>D25+0.1</f>
+        <v>2.5000000000000009</v>
+      </c>
+      <c r="E26" s="10">
+        <f t="shared" si="0"/>
+        <v>2.100000000000001</v>
+      </c>
+      <c r="F26" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G26" s="10">
+        <v>1.702093577478081E-4</v>
+      </c>
+      <c r="H26" s="10">
+        <v>1.7164925520773977E-4</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="10">
+        <f t="shared" si="1"/>
+        <v>7.0496391374728212E-3</v>
+      </c>
+      <c r="K26" s="8"/>
+      <c r="L26" s="10">
+        <f t="shared" si="2"/>
+        <v>141.85123245308176</v>
+      </c>
+      <c r="M26" s="8"/>
+      <c r="N26" s="10">
+        <f t="shared" si="3"/>
+        <v>1.1999145499430607E-6</v>
+      </c>
+      <c r="O26" s="8"/>
+      <c r="P26" s="10">
+        <f t="shared" si="4"/>
+        <v>833392.67787648109</v>
+      </c>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="10">
+        <f t="shared" si="5"/>
+        <v>734389.7048551651</v>
+      </c>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="10">
+        <v>2.0499999523162842</v>
+      </c>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="10">
+        <v>1.2441426224540919E-4</v>
+      </c>
+      <c r="Z26" s="8"/>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C27" s="8"/>
+      <c r="D27" s="10">
+        <f>D26+0.1</f>
+        <v>2.600000000000001</v>
+      </c>
+      <c r="E27" s="10">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000011</v>
+      </c>
+      <c r="F27" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G27" s="10">
+        <v>1.8473727686796337E-4</v>
+      </c>
+      <c r="H27" s="10">
+        <v>1.8616307352203876E-4</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="10">
+        <f t="shared" si="1"/>
+        <v>7.0163358386980124E-3</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="L27" s="10">
+        <f t="shared" si="2"/>
+        <v>142.52453459889759</v>
+      </c>
+      <c r="M27" s="8"/>
+      <c r="N27" s="10">
+        <f t="shared" si="3"/>
+        <v>1.2961787764321688E-6</v>
+      </c>
+      <c r="O27" s="8"/>
+      <c r="P27" s="10">
+        <f t="shared" si="4"/>
+        <v>771498.51408042375</v>
+      </c>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="10">
+        <f t="shared" si="5"/>
+        <v>676636.58423059259</v>
+      </c>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="10">
+        <v>2.1500000953674316</v>
+      </c>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="10">
+        <v>1.2918858556076884E-4</v>
+      </c>
+      <c r="Z27" s="8"/>
+    </row>
+    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C28" s="8"/>
+      <c r="D28" s="10">
+        <f>D27+0.1</f>
+        <v>2.7000000000000011</v>
+      </c>
+      <c r="E28" s="10">
+        <f t="shared" si="0"/>
+        <v>2.3000000000000012</v>
+      </c>
+      <c r="F28" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G28" s="10">
+        <v>1.9960060308221728E-4</v>
+      </c>
+      <c r="H28" s="10">
+        <v>2.0099880930501968E-4</v>
+      </c>
+      <c r="I28" s="8"/>
+      <c r="J28" s="10">
+        <f t="shared" si="1"/>
+        <v>7.0050200310590683E-3</v>
+      </c>
+      <c r="K28" s="8"/>
+      <c r="L28" s="10">
+        <f t="shared" si="2"/>
+        <v>142.75476666250344</v>
+      </c>
+      <c r="M28" s="8"/>
+      <c r="N28" s="10">
+        <f t="shared" si="3"/>
+        <v>1.3982062228024025E-6</v>
+      </c>
+      <c r="O28" s="8"/>
+      <c r="P28" s="10">
+        <f t="shared" si="4"/>
+        <v>715202.08084592549</v>
+      </c>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="10">
+        <f t="shared" si="5"/>
+        <v>626250.61282260448</v>
+      </c>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="10">
+        <v>2.25</v>
+      </c>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="10">
+        <v>1.3364623009692878E-4</v>
+      </c>
+      <c r="Z28" s="8"/>
+    </row>
+    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C29" s="8"/>
+      <c r="D29" s="10">
+        <f>D28+0.1</f>
+        <v>2.8000000000000012</v>
+      </c>
+      <c r="E29" s="10">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000012</v>
+      </c>
+      <c r="F29" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G29" s="10">
+        <v>2.1477586415130645E-4</v>
+      </c>
+      <c r="H29" s="10">
+        <v>2.1613189892377704E-4</v>
+      </c>
+      <c r="I29" s="8"/>
+      <c r="J29" s="10">
+        <f t="shared" si="1"/>
+        <v>7.0152449796856801E-3</v>
+      </c>
+      <c r="K29" s="8"/>
+      <c r="L29" s="10">
+        <f t="shared" si="2"/>
+        <v>142.54669692872298</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="10">
+        <f t="shared" si="3"/>
+        <v>1.5067053027451062E-6</v>
+      </c>
+      <c r="O29" s="8"/>
+      <c r="P29" s="10">
+        <f t="shared" si="4"/>
+        <v>663699.79463009362</v>
+      </c>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="8"/>
+      <c r="T29" s="10">
+        <f t="shared" si="5"/>
+        <v>582002.08153714763</v>
+      </c>
+      <c r="U29" s="8"/>
+      <c r="V29" s="8"/>
+      <c r="W29" s="10">
+        <v>2.3499999046325684</v>
+      </c>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="10">
+        <v>1.378019223921001E-4</v>
+      </c>
+      <c r="Z29" s="8"/>
+    </row>
+    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C30" s="8"/>
+      <c r="D30" s="10">
+        <f>D29+0.1</f>
+        <v>2.9000000000000012</v>
+      </c>
+      <c r="E30" s="10">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000013</v>
+      </c>
+      <c r="F30" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G30" s="10">
+        <v>2.3024117399472743E-4</v>
+      </c>
+      <c r="H30" s="10">
+        <v>2.3153919028118253E-4</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="10">
+        <f t="shared" si="1"/>
+        <v>7.0470469287392855E-3</v>
+      </c>
+      <c r="K30" s="8"/>
+      <c r="L30" s="10">
+        <f t="shared" si="2"/>
+        <v>141.90341147322255</v>
+      </c>
+      <c r="M30" s="8"/>
+      <c r="N30" s="10">
+        <f t="shared" si="3"/>
+        <v>1.6225203580688715E-6</v>
+      </c>
+      <c r="O30" s="8"/>
+      <c r="P30" s="10">
+        <f t="shared" si="4"/>
+        <v>616325.08647854684</v>
+      </c>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="10">
+        <f t="shared" si="5"/>
+        <v>542908.97597170225</v>
+      </c>
+      <c r="U30" s="8"/>
+      <c r="V30" s="8"/>
+      <c r="W30" s="10">
+        <v>2.4500000476837158</v>
+      </c>
+      <c r="X30" s="8"/>
+      <c r="Y30" s="10">
+        <v>1.4167452172841877E-4</v>
+      </c>
+      <c r="Z30" s="8"/>
+    </row>
+    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C31" s="8"/>
+      <c r="D31" s="10">
+        <f>D30+0.1</f>
+        <v>3.0000000000000013</v>
+      </c>
+      <c r="E31" s="10">
+        <f t="shared" si="0"/>
+        <v>2.6000000000000014</v>
+      </c>
+      <c r="F31" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G31" s="10">
+        <v>2.4597617448307574E-4</v>
+      </c>
+      <c r="H31" s="10">
+        <v>2.4719879729673266E-4</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="10">
+        <f t="shared" si="1"/>
+        <v>7.1007040546932024E-3</v>
+      </c>
+      <c r="K31" s="8"/>
+      <c r="L31" s="10">
+        <f t="shared" si="2"/>
+        <v>140.83110523935315</v>
+      </c>
+      <c r="M31" s="8"/>
+      <c r="N31" s="10">
+        <f t="shared" si="3"/>
+        <v>1.7466040195098986E-6</v>
+      </c>
+      <c r="O31" s="8"/>
+      <c r="P31" s="10">
+        <f t="shared" si="4"/>
+        <v>572539.61907210224</v>
+      </c>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="10">
+        <f t="shared" si="5"/>
+        <v>508179.29932722228</v>
+      </c>
+      <c r="U31" s="8"/>
+      <c r="V31" s="8"/>
+      <c r="W31" s="10">
+        <v>2.5499999523162842</v>
+      </c>
+      <c r="X31" s="8"/>
+      <c r="Y31" s="10">
+        <v>1.4527933672070503E-4</v>
+      </c>
+      <c r="Z31" s="8"/>
+    </row>
+    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C32" s="8"/>
+      <c r="D32" s="10">
+        <f>D31+0.1</f>
+        <v>3.1000000000000014</v>
+      </c>
+      <c r="E32" s="10">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000015</v>
+      </c>
+      <c r="F32" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G32" s="10">
+        <v>2.6196203543804586E-4</v>
+      </c>
+      <c r="H32" s="10">
+        <v>2.6309004169888794E-4</v>
+      </c>
+      <c r="I32" s="8"/>
+      <c r="J32" s="10">
+        <f t="shared" si="1"/>
+        <v>7.1766522641080821E-3</v>
+      </c>
+      <c r="K32" s="8"/>
+      <c r="L32" s="10">
+        <f t="shared" si="2"/>
+        <v>139.34073481603758</v>
+      </c>
+      <c r="M32" s="8"/>
+      <c r="N32" s="10">
+        <f t="shared" si="3"/>
+        <v>1.8800104347368134E-6</v>
+      </c>
+      <c r="O32" s="8"/>
+      <c r="P32" s="10">
+        <f t="shared" si="4"/>
+        <v>531911.94129727909</v>
+      </c>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="10">
+        <f t="shared" si="5"/>
+        <v>477168.37972715538</v>
+      </c>
+      <c r="U32" s="8"/>
+      <c r="V32" s="8"/>
+      <c r="W32" s="10">
+        <v>2.6500000953674316</v>
+      </c>
+      <c r="X32" s="8"/>
+      <c r="Y32" s="10">
+        <v>1.486330438638106E-4</v>
+      </c>
+      <c r="Z32" s="8"/>
+    </row>
+    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C33" s="8"/>
+      <c r="D33" s="10">
+        <f>D32+0.1</f>
+        <v>3.2000000000000015</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000016</v>
+      </c>
+      <c r="F33" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G33" s="10">
+        <v>2.7818130911327899E-4</v>
+      </c>
+      <c r="H33" s="10">
+        <v>2.7919336571358144E-4</v>
+      </c>
+      <c r="I33" s="8"/>
+      <c r="J33" s="10">
+        <f t="shared" si="1"/>
+        <v>7.2762372391477889E-3</v>
+      </c>
+      <c r="K33" s="8"/>
+      <c r="L33" s="10">
+        <f t="shared" si="2"/>
+        <v>137.43367170874743</v>
+      </c>
+      <c r="M33" s="8"/>
+      <c r="N33" s="10">
+        <f t="shared" si="3"/>
+        <v>2.0241132006049228E-6</v>
+      </c>
+      <c r="O33" s="8"/>
+      <c r="P33" s="10">
+        <f t="shared" si="4"/>
+        <v>494043.5148099137</v>
+      </c>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="10">
+        <f t="shared" si="5"/>
+        <v>449347.22752741957</v>
+      </c>
+      <c r="U33" s="8"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="10">
+        <v>2.75</v>
+      </c>
+      <c r="X33" s="8"/>
+      <c r="Y33" s="10">
+        <v>1.5175275621004403E-4</v>
+      </c>
+      <c r="Z33" s="8"/>
+    </row>
+    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C34" s="8"/>
+      <c r="D34" s="10">
+        <f>D33+0.1</f>
+        <v>3.3000000000000016</v>
+      </c>
+      <c r="E34" s="10">
+        <f t="shared" si="0"/>
+        <v>2.9000000000000017</v>
+      </c>
+      <c r="F34" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="G34" s="10">
+        <v>2.94617930194363E-4</v>
+      </c>
+      <c r="H34" s="10">
+        <v>2.9549011378549039E-4</v>
+      </c>
+      <c r="I34" s="8"/>
+      <c r="J34" s="10">
+        <f t="shared" si="1"/>
+        <v>7.4009717479856848E-3</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="L34" s="10">
+        <f t="shared" si="2"/>
+        <v>135.11739188467635</v>
+      </c>
+      <c r="M34" s="8"/>
+      <c r="N34" s="10">
+        <f t="shared" si="3"/>
+        <v>2.1804589778184992E-6</v>
+      </c>
+      <c r="O34" s="8"/>
+      <c r="P34" s="10">
+        <f t="shared" si="4"/>
+        <v>458619.03854778217</v>
+      </c>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="10">
+        <f t="shared" si="5"/>
+        <v>424278.31842256169</v>
+      </c>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="10">
+        <v>2.8499999046325684</v>
+      </c>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="10">
+        <v>1.546528801554814E-4</v>
+      </c>
+      <c r="Z34" s="8"/>
+    </row>
+    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C35" s="8"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="10">
+        <v>2.9500000476837158</v>
+      </c>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="10">
+        <v>1.5735015040263534E-4</v>
+      </c>
+      <c r="Z35" s="8"/>
+    </row>
+    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="10">
+        <v>3.0499999523162842</v>
+      </c>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="10">
+        <v>1.598587550688535E-4</v>
+      </c>
+      <c r="Z36" s="8"/>
+    </row>
+    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="10">
+        <v>3.1500000953674316</v>
+      </c>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="10">
+        <v>1.621925039216876E-4</v>
+      </c>
+      <c r="Z37" s="8"/>
+    </row>
+    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="10">
+        <v>3.25</v>
+      </c>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="10">
+        <v>1.6436637088190764E-4</v>
+      </c>
+      <c r="Z38" s="8"/>
+    </row>
+    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
aggiunti dati su excel ricavati dal circuito imponendo GVO e potenza
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E090AC3-12BD-49DC-B7C6-D00FCF8A0E84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD9CE9A-4586-407C-AB44-DADF087BA270}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
   <si>
     <t>Ib</t>
   </si>
@@ -161,13 +161,172 @@
   </si>
   <si>
     <t>PMOS</t>
+  </si>
+  <si>
+    <t>(Ro2 || Ro4) * gm2</t>
+  </si>
+  <si>
+    <t>Ro2</t>
+  </si>
+  <si>
+    <t>Ro4</t>
+  </si>
+  <si>
+    <t>gm2</t>
+  </si>
+  <si>
+    <t>R02 || Ro4</t>
+  </si>
+  <si>
+    <t>Vgs_M2</t>
+  </si>
+  <si>
+    <t>Vgs_M4</t>
+  </si>
+  <si>
+    <t>Av1_dd primo stadio</t>
+  </si>
+  <si>
+    <t>Av1_dd</t>
+  </si>
+  <si>
+    <t>calcolato</t>
+  </si>
+  <si>
+    <t>risultante da pspice</t>
+  </si>
+  <si>
+    <t>Noi abbiamo che (W6/L6)/(W4/L4) *1/2 = (W7/L7)/(W5/L5)</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Vgs_M6</t>
+  </si>
+  <si>
+    <t>Valori R</t>
+  </si>
+  <si>
+    <t>Vs</t>
+  </si>
+  <si>
+    <t>Valori circuito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrente ref uA </t>
+  </si>
+  <si>
+    <t>IdMB (teo)</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>P_hp</t>
+  </si>
+  <si>
+    <t>I_ref</t>
+  </si>
+  <si>
+    <t>I_out</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>GVO</t>
+  </si>
+  <si>
+    <t>Va</t>
+  </si>
+  <si>
+    <t>massimo per avere guadagno desiderato</t>
+  </si>
+  <si>
+    <t>I_MB</t>
+  </si>
+  <si>
+    <t>GVO!</t>
+  </si>
+  <si>
+    <t>GVO scelto, deve essere inferiore al massimo</t>
+  </si>
+  <si>
+    <t>I_5</t>
+  </si>
+  <si>
+    <t>I_B</t>
+  </si>
+  <si>
+    <t>I_3</t>
+  </si>
+  <si>
+    <t>I_4</t>
+  </si>
+  <si>
+    <t>I_1</t>
+  </si>
+  <si>
+    <t>I_2</t>
+  </si>
+  <si>
+    <t>I_6</t>
+  </si>
+  <si>
+    <t>I_7</t>
+  </si>
+  <si>
+    <t>W/L_MB</t>
+  </si>
+  <si>
+    <t>W/L_5</t>
+  </si>
+  <si>
+    <t>W/L_3</t>
+  </si>
+  <si>
+    <t>W/L_4</t>
+  </si>
+  <si>
+    <t>W/L_2</t>
+  </si>
+  <si>
+    <t>W/L_1</t>
+  </si>
+  <si>
+    <t>W/L_6</t>
+  </si>
+  <si>
+    <t>W/L_7</t>
+  </si>
+  <si>
+    <t>potenza calcolata con correnti imposte</t>
+  </si>
+  <si>
+    <t>approx per ecc</t>
+  </si>
+  <si>
+    <t>W transistor</t>
+  </si>
+  <si>
+    <t>I_risultante</t>
+  </si>
+  <si>
+    <t>R= 242,3K</t>
+  </si>
+  <si>
+    <t>per costruz</t>
+  </si>
+  <si>
+    <t>GVO_risultante</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +352,15 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -232,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -248,6 +416,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2775,10 +2946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P183"/>
+  <dimension ref="B2:Q183"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2786,8 +2957,11 @@
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
     <col min="14" max="14" width="21.140625" customWidth="1"/>
     <col min="16" max="16" width="28.85546875" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
@@ -2796,13 +2970,16 @@
       </c>
       <c r="G2">
         <f>C6*(N16/N6)</f>
-        <v>1.4999999999999999E-4</v>
+        <v>5.9000000000000003E-6</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="P3" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2816,7 +2993,7 @@
       </c>
       <c r="G4">
         <f>-(ABS(C10)+SQRT(2*C6/C18))</f>
-        <v>-2.826271987040891</v>
+        <v>-1.1152823312836488</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>20</v>
@@ -2830,15 +3007,15 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <f>150*POWER(10,-6)</f>
-        <v>1.4999999999999999E-4</v>
+        <f>5.9*POWER(10,-6)</f>
+        <v>5.9000000000000003E-6</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G6">
         <f>(C4+G4)/G2</f>
-        <v>3158.1867530607256</v>
+        <v>370291.13029090688</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>13</v>
@@ -2894,7 +3071,7 @@
       </c>
       <c r="G10">
         <f>C6/2</f>
-        <v>7.4999999999999993E-5</v>
+        <v>2.9500000000000001E-6</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>15</v>
@@ -2925,7 +3102,7 @@
       </c>
       <c r="G12">
         <f>C6/2</f>
-        <v>7.4999999999999993E-5</v>
+        <v>2.9500000000000001E-6</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>16</v>
@@ -2940,6 +3117,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="P12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K13" s="2"/>
@@ -2957,7 +3137,7 @@
       </c>
       <c r="G14">
         <f>G12*N12/N10</f>
-        <v>7.4999999999999993E-5</v>
+        <v>2.9500000000000001E-6</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>17</v>
@@ -2989,7 +3169,7 @@
       </c>
       <c r="G16">
         <f>N14/N16*C6</f>
-        <v>1.4999999999999999E-4</v>
+        <v>5.9000000000000003E-6</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>18</v>
@@ -3005,7 +3185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -3013,6 +3193,528 @@
         <f>C14*N6</f>
         <v>6.586000000000001E-5</v>
       </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21">
+        <f>(G16+G12+G10+C6)*C4</f>
+        <v>5.8409999999999998E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="14">
+        <v>30</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="14">
+        <v>20000</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="M24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="M25">
+        <v>50</v>
+      </c>
+      <c r="N25">
+        <v>55.05</v>
+      </c>
+      <c r="O25">
+        <v>13757</v>
+      </c>
+      <c r="P25">
+        <v>1.996</v>
+      </c>
+      <c r="Q25">
+        <f>-P25</f>
+        <v>-1.996</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="14">
+        <v>10</v>
+      </c>
+      <c r="M26">
+        <v>10</v>
+      </c>
+      <c r="N26">
+        <v>16.02</v>
+      </c>
+      <c r="O26">
+        <v>102845</v>
+      </c>
+      <c r="P26">
+        <v>1.397</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26:Q31" si="1">-P26</f>
+        <v>-1.397</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="14">
+        <v>20</v>
+      </c>
+      <c r="N27">
+        <v>9.3710000000000004</v>
+      </c>
+      <c r="O27">
+        <v>200000</v>
+      </c>
+      <c r="P27">
+        <v>1.234</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="1"/>
+        <v>-1.234</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="14">
+        <v>20</v>
+      </c>
+      <c r="N28">
+        <v>46.32</v>
+      </c>
+      <c r="O28">
+        <v>20000</v>
+      </c>
+      <c r="P28">
+        <v>1.9019999999999999</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="1"/>
+        <v>-1.9019999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="N29">
+        <v>7.7560000000000002</v>
+      </c>
+      <c r="O29">
+        <v>250000</v>
+      </c>
+      <c r="P29">
+        <v>1.1870000000000001</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>-1.1870000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="14">
+        <f>(C27+C28+C26)*C25</f>
+        <v>165</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="M30">
+        <v>30</v>
+      </c>
+      <c r="N30">
+        <v>39</v>
+      </c>
+      <c r="O30">
+        <v>27558</v>
+      </c>
+      <c r="P30">
+        <v>1.8029999999999999</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="1"/>
+        <v>-1.8029999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31">
+        <f>C23/SQRT(C24)</f>
+        <v>0.21213203435596426</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="M31">
+        <v>5.9</v>
+      </c>
+      <c r="N31">
+        <v>10</v>
+      </c>
+      <c r="O31">
+        <v>185000</v>
+      </c>
+      <c r="P31">
+        <v>1.2509999999999999</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>-1.2509999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34">
+        <v>0.15</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="H35" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="N35" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36">
+        <f>C26</f>
+        <v>10</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36">
+        <f>2*C36*POWER(10,-6)/($C$14*$C$34*$C$34)</f>
+        <v>13.496642710125853</v>
+      </c>
+      <c r="H36">
+        <f>ROUNDUP(F36,0)</f>
+        <v>14</v>
+      </c>
+      <c r="J36">
+        <f>1.4*H36</f>
+        <v>19.599999999999998</v>
+      </c>
+      <c r="L36">
+        <v>10</v>
+      </c>
+      <c r="N36">
+        <v>0.185</v>
+      </c>
+      <c r="O36">
+        <v>-0.877</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37">
+        <f>C27</f>
+        <v>20</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37">
+        <f t="shared" ref="F37:F43" si="2">2*C37*POWER(10,-6)/($C$14*$C$34*$C$34)</f>
+        <v>26.993285420251706</v>
+      </c>
+      <c r="H37">
+        <f t="shared" ref="H37:H43" si="3">ROUNDUP(F37,0)</f>
+        <v>27</v>
+      </c>
+      <c r="J37">
+        <f>1.4*H37</f>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="L37">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="N37">
+        <v>0.185</v>
+      </c>
+      <c r="O37">
+        <v>-0.877</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38">
+        <f>C27/2</f>
+        <v>10</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38">
+        <f>2*C38*POWER(10,-6)/($C$16*$C$34*$C$34)</f>
+        <v>4.0952053335954268</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J38">
+        <f>1.4*H38</f>
+        <v>7</v>
+      </c>
+      <c r="L38">
+        <v>10.18</v>
+      </c>
+      <c r="N38">
+        <v>0.187</v>
+      </c>
+      <c r="O38">
+        <v>0.68500000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39">
+        <f>C27/2</f>
+        <v>10</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39">
+        <f>2*C39*POWER(10,-6)/($C$16*$C$34*$C$34)</f>
+        <v>4.0952053335954268</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <f>1.4*H39</f>
+        <v>7</v>
+      </c>
+      <c r="L39">
+        <v>10.18</v>
+      </c>
+      <c r="N39">
+        <v>0.187</v>
+      </c>
+      <c r="O39">
+        <v>0.68500000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40">
+        <f>C27/2</f>
+        <v>10</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>13.496642710125853</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J40">
+        <f>1.4*H40</f>
+        <v>19.599999999999998</v>
+      </c>
+      <c r="L40">
+        <v>10.18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41">
+        <f>C27/2</f>
+        <v>10</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>13.496642710125853</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="J41">
+        <f>1.4*H41</f>
+        <v>19.599999999999998</v>
+      </c>
+      <c r="L41">
+        <v>10.18</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42">
+        <f>C28</f>
+        <v>20</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42">
+        <f>2*C42*POWER(10,-6)/($C$16*$C$34*$C$34)</f>
+        <v>8.1904106671908536</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H42">
+        <v>10</v>
+      </c>
+      <c r="J42">
+        <f>1.4*H42</f>
+        <v>14</v>
+      </c>
+      <c r="L42">
+        <v>20.43</v>
+      </c>
+      <c r="N42">
+        <v>0.187</v>
+      </c>
+      <c r="O42">
+        <v>0.68500000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43">
+        <f>C28</f>
+        <v>20</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43">
+        <f>2*C43*POWER(10,-6)/($C$14*$C$34*$C$34)</f>
+        <v>26.993285420251706</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="J43">
+        <f>1.4*H43</f>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="L43">
+        <v>20.43</v>
+      </c>
+      <c r="N43">
+        <v>0.185</v>
+      </c>
+      <c r="O43">
+        <v>-0.877</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
@@ -3386,10 +4088,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E533CDB7-452E-4AEE-B021-5A11B297142C}">
-  <dimension ref="B3:Z77"/>
+  <dimension ref="B3:Z93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="N90" sqref="N90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,11 +4101,13 @@
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:26" x14ac:dyDescent="0.25">
@@ -5422,7 +6126,7 @@
         <v>0.7</v>
       </c>
       <c r="E43">
-        <f>D43-0.692</f>
+        <f t="shared" ref="E43:E69" si="7">D43-0.692</f>
         <v>8.0000000000000071E-3</v>
       </c>
       <c r="F43">
@@ -5436,28 +6140,33 @@
       </c>
       <c r="I43" s="11"/>
       <c r="J43">
-        <f>((H43-G43)/(F43-E43))/G43</f>
+        <f t="shared" ref="J43:J69" si="8">((H43-G43)/(F43-E43))/G43</f>
         <v>9.2328763826457615E-3</v>
       </c>
       <c r="K43" s="11"/>
       <c r="L43">
-        <f>1/J43</f>
+        <f t="shared" ref="L43:L69" si="9">1/J43</f>
         <v>108.30860920867666</v>
       </c>
       <c r="M43" s="11"/>
       <c r="N43" s="3">
-        <f>((H43-G43)/(F43-E43))</f>
+        <f t="shared" ref="N43:N69" si="10">((H43-G43)/(F43-E43))</f>
         <v>1.4963270261026754E-10</v>
       </c>
       <c r="O43" s="11"/>
       <c r="P43">
-        <f>1/N43</f>
+        <f t="shared" ref="P43:P69" si="11">1/N43</f>
         <v>6683031065.7730627</v>
       </c>
       <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
+      <c r="R43" s="10">
+        <v>200</v>
+      </c>
       <c r="S43" s="11"/>
-      <c r="T43" s="11"/>
+      <c r="T43" s="13">
+        <f>$R$43/G43</f>
+        <v>12340719938.332809</v>
+      </c>
       <c r="U43" s="11"/>
       <c r="V43" s="11"/>
       <c r="W43" s="10">
@@ -5473,11 +6182,11 @@
       <c r="B44" s="3"/>
       <c r="C44" s="11"/>
       <c r="D44">
-        <f>D43+0.1</f>
+        <f t="shared" ref="D44:D69" si="12">D43+0.1</f>
         <v>0.79999999999999993</v>
       </c>
       <c r="E44">
-        <f>D44-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.10799999999999998</v>
       </c>
       <c r="F44">
@@ -5491,28 +6200,31 @@
       </c>
       <c r="I44" s="11"/>
       <c r="J44">
-        <f>((H44-G44)/(F44-E44))/G44</f>
+        <f t="shared" si="8"/>
         <v>8.4961166225202452E-3</v>
       </c>
       <c r="K44" s="11"/>
       <c r="L44">
-        <f>1/J44</f>
+        <f t="shared" si="9"/>
         <v>117.70083256029565</v>
       </c>
       <c r="M44" s="11"/>
       <c r="N44">
-        <f>((H44-G44)/(F44-E44))</f>
+        <f t="shared" si="10"/>
         <v>1.1393570576002486E-9</v>
       </c>
       <c r="O44" s="11"/>
       <c r="P44">
-        <f>1/N44</f>
+        <f t="shared" si="11"/>
         <v>877687984.92917836</v>
       </c>
       <c r="Q44" s="11"/>
       <c r="R44" s="11"/>
       <c r="S44" s="11"/>
-      <c r="T44" s="11"/>
+      <c r="T44" s="13">
+        <f t="shared" ref="T44:T69" si="13">$R$43/G44</f>
+        <v>1491387895.628618</v>
+      </c>
       <c r="U44" s="11"/>
       <c r="V44" s="11"/>
       <c r="W44" s="10">
@@ -5528,11 +6240,11 @@
       <c r="B45" s="3"/>
       <c r="C45" s="11"/>
       <c r="D45">
-        <f>D44+0.1</f>
+        <f t="shared" si="12"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="E45">
-        <f>D45-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.20799999999999996</v>
       </c>
       <c r="F45">
@@ -5546,28 +6258,31 @@
       </c>
       <c r="I45" s="11"/>
       <c r="J45">
-        <f>((H45-G45)/(F45-E45))/G45</f>
+        <f t="shared" si="8"/>
         <v>7.906931105712273E-3</v>
       </c>
       <c r="K45" s="11"/>
       <c r="L45">
-        <f>1/J45</f>
+        <f t="shared" si="9"/>
         <v>126.47131821821002</v>
       </c>
       <c r="M45" s="11"/>
       <c r="N45">
-        <f>((H45-G45)/(F45-E45))</f>
+        <f t="shared" si="10"/>
         <v>4.5691115114517988E-9</v>
       </c>
       <c r="O45" s="11"/>
       <c r="P45">
-        <f>1/N45</f>
+        <f t="shared" si="11"/>
         <v>218860931.16651863</v>
       </c>
       <c r="Q45" s="11"/>
       <c r="R45" s="11"/>
       <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
+      <c r="T45" s="13">
+        <f t="shared" si="13"/>
+        <v>346103660.89313972</v>
+      </c>
       <c r="U45" s="11"/>
       <c r="V45" s="11"/>
       <c r="W45" s="10">
@@ -5583,11 +6298,11 @@
       <c r="B46" s="3"/>
       <c r="C46" s="11"/>
       <c r="D46">
-        <f>D45+0.1</f>
+        <f t="shared" si="12"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="E46">
-        <f>D46-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.30799999999999994</v>
       </c>
       <c r="F46">
@@ -5601,28 +6316,31 @@
       </c>
       <c r="I46" s="11"/>
       <c r="J46">
-        <f>((H46-G46)/(F46-E46))/G46</f>
+        <f t="shared" si="8"/>
         <v>7.5257072572212352E-3</v>
       </c>
       <c r="K46" s="11"/>
       <c r="L46">
-        <f>1/J46</f>
+        <f t="shared" si="9"/>
         <v>132.87787656641277</v>
       </c>
       <c r="M46" s="11"/>
       <c r="N46">
-        <f>((H46-G46)/(F46-E46))</f>
+        <f t="shared" si="10"/>
         <v>1.1000721427075573E-8</v>
       </c>
       <c r="O46" s="11"/>
       <c r="P46">
-        <f>1/N46</f>
+        <f t="shared" si="11"/>
         <v>90903129.092856199</v>
       </c>
       <c r="Q46" s="11"/>
       <c r="R46" s="11"/>
       <c r="S46" s="11"/>
-      <c r="T46" s="11"/>
+      <c r="T46" s="13">
+        <f t="shared" si="13"/>
+        <v>136822067.66364533</v>
+      </c>
       <c r="U46" s="11"/>
       <c r="V46" s="11"/>
       <c r="W46" s="10">
@@ -5638,11 +6356,11 @@
       <c r="B47" s="3"/>
       <c r="C47" s="11"/>
       <c r="D47">
-        <f>D46+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.0999999999999999</v>
       </c>
       <c r="E47">
-        <f>D47-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.40799999999999992</v>
       </c>
       <c r="F47">
@@ -5656,28 +6374,31 @@
       </c>
       <c r="I47" s="11"/>
       <c r="J47">
-        <f>((H47-G47)/(F47-E47))/G47</f>
+        <f t="shared" si="8"/>
         <v>7.2492450609443013E-3</v>
       </c>
       <c r="K47" s="11"/>
       <c r="L47">
-        <f>1/J47</f>
+        <f t="shared" si="9"/>
         <v>137.94539867158772</v>
       </c>
       <c r="M47" s="11"/>
       <c r="N47">
-        <f>((H47-G47)/(F47-E47))</f>
+        <f t="shared" si="10"/>
         <v>1.9992451524007526E-8</v>
       </c>
       <c r="O47" s="11"/>
       <c r="P47">
-        <f>1/N47</f>
+        <f t="shared" si="11"/>
         <v>50018878.315106601</v>
       </c>
       <c r="Q47" s="11"/>
       <c r="R47" s="11"/>
       <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
+      <c r="T47" s="13">
+        <f t="shared" si="13"/>
+        <v>72519821.315952107</v>
+      </c>
       <c r="U47" s="11"/>
       <c r="V47" s="11"/>
       <c r="W47" s="10">
@@ -5693,11 +6414,11 @@
       <c r="B48" s="3"/>
       <c r="C48" s="11"/>
       <c r="D48">
-        <f>D47+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.2</v>
       </c>
       <c r="E48">
-        <f>D48-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.50800000000000001</v>
       </c>
       <c r="F48">
@@ -5711,28 +6432,31 @@
       </c>
       <c r="I48" s="11"/>
       <c r="J48">
-        <f>((H48-G48)/(F48-E48))/G48</f>
+        <f t="shared" si="8"/>
         <v>7.008349023358341E-3</v>
       </c>
       <c r="K48" s="11"/>
       <c r="L48">
-        <f>1/J48</f>
+        <f t="shared" si="9"/>
         <v>142.68695760828541</v>
       </c>
       <c r="M48" s="11"/>
       <c r="N48">
-        <f>((H48-G48)/(F48-E48))</f>
+        <f t="shared" si="10"/>
         <v>3.107527097791199E-8</v>
       </c>
       <c r="O48" s="11"/>
       <c r="P48">
-        <f>1/N48</f>
+        <f t="shared" si="11"/>
         <v>32179928.558331497</v>
       </c>
       <c r="Q48" s="11"/>
       <c r="R48" s="11"/>
       <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
+      <c r="T48" s="13">
+        <f t="shared" si="13"/>
+        <v>45105634.176704742</v>
+      </c>
       <c r="U48" s="11"/>
       <c r="V48" s="11"/>
       <c r="W48" s="10">
@@ -5748,11 +6472,11 @@
       <c r="B49" s="3"/>
       <c r="C49" s="11"/>
       <c r="D49">
-        <f>D48+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.3</v>
       </c>
       <c r="E49">
-        <f>D49-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.6080000000000001</v>
       </c>
       <c r="F49">
@@ -5766,28 +6490,31 @@
       </c>
       <c r="I49" s="11"/>
       <c r="J49">
-        <f>((H49-G49)/(F49-E49))/G49</f>
+        <f t="shared" si="8"/>
         <v>6.7734835595249267E-3</v>
       </c>
       <c r="K49" s="11"/>
       <c r="L49">
-        <f>1/J49</f>
+        <f t="shared" si="9"/>
         <v>147.63452088014475</v>
       </c>
       <c r="M49" s="11"/>
       <c r="N49">
-        <f>((H49-G49)/(F49-E49))</f>
+        <f t="shared" si="10"/>
         <v>4.3828894286385652E-8</v>
       </c>
       <c r="O49" s="11"/>
       <c r="P49">
-        <f>1/N49</f>
+        <f t="shared" si="11"/>
         <v>22815998.81269706</v>
       </c>
       <c r="Q49" s="11"/>
       <c r="R49" s="11"/>
       <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
+      <c r="T49" s="13">
+        <f>$R$43/G49</f>
+        <v>30908758.570388757</v>
+      </c>
       <c r="U49" s="11"/>
       <c r="V49" s="11"/>
       <c r="W49" s="10">
@@ -5803,11 +6530,11 @@
       <c r="B50" s="3"/>
       <c r="C50" s="11"/>
       <c r="D50">
-        <f>D49+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.4000000000000001</v>
       </c>
       <c r="E50">
-        <f>D50-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.70800000000000018</v>
       </c>
       <c r="F50">
@@ -5821,28 +6548,31 @@
       </c>
       <c r="I50" s="11"/>
       <c r="J50">
-        <f>((H50-G50)/(F50-E50))/G50</f>
+        <f t="shared" si="8"/>
         <v>6.5304732789656199E-3</v>
       </c>
       <c r="K50" s="11"/>
       <c r="L50">
-        <f>1/J50</f>
+        <f t="shared" si="9"/>
         <v>153.12825844046526</v>
       </c>
       <c r="M50" s="11"/>
       <c r="N50">
-        <f>((H50-G50)/(F50-E50))</f>
+        <f t="shared" si="10"/>
         <v>5.7805546357824399E-8</v>
       </c>
       <c r="O50" s="11"/>
       <c r="P50">
-        <f>1/N50</f>
+        <f t="shared" si="11"/>
         <v>17299378.052926973</v>
       </c>
       <c r="Q50" s="11"/>
       <c r="R50" s="11"/>
       <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
+      <c r="T50" s="13">
+        <f t="shared" si="13"/>
+        <v>22594625.223472774</v>
+      </c>
       <c r="U50" s="11"/>
       <c r="V50" s="11"/>
       <c r="W50" s="10">
@@ -5858,11 +6588,11 @@
       <c r="B51" s="3"/>
       <c r="C51" s="11"/>
       <c r="D51">
-        <f>D50+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.5000000000000002</v>
       </c>
       <c r="E51">
-        <f>D51-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.80800000000000027</v>
       </c>
       <c r="F51">
@@ -5876,28 +6606,31 @@
       </c>
       <c r="I51" s="11"/>
       <c r="J51">
-        <f>((H51-G51)/(F51-E51))/G51</f>
+        <f t="shared" si="8"/>
         <v>6.2705100945088452E-3</v>
       </c>
       <c r="K51" s="11"/>
       <c r="L51">
-        <f>1/J51</f>
+        <f t="shared" si="9"/>
         <v>159.47665898436412</v>
       </c>
       <c r="M51" s="11"/>
       <c r="N51">
-        <f>((H51-G51)/(F51-E51))</f>
+        <f t="shared" si="10"/>
         <v>7.2496435820826574E-8</v>
       </c>
       <c r="O51" s="11"/>
       <c r="P51">
-        <f>1/N51</f>
+        <f t="shared" si="11"/>
         <v>13793781.56564109</v>
       </c>
       <c r="Q51" s="11"/>
       <c r="R51" s="11"/>
       <c r="S51" s="11"/>
-      <c r="T51" s="11"/>
+      <c r="T51" s="13">
+        <f t="shared" si="13"/>
+        <v>17298809.309760496</v>
+      </c>
       <c r="U51" s="11"/>
       <c r="V51" s="11"/>
       <c r="W51" s="10">
@@ -5913,11 +6646,11 @@
       <c r="B52" s="3"/>
       <c r="C52" s="11"/>
       <c r="D52">
-        <f>D51+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.6000000000000003</v>
       </c>
       <c r="E52">
-        <f>D52-0.692</f>
+        <f t="shared" si="7"/>
         <v>0.90800000000000036</v>
       </c>
       <c r="F52">
@@ -5931,28 +6664,31 @@
       </c>
       <c r="I52" s="11"/>
       <c r="J52">
-        <f>((H52-G52)/(F52-E52))/G52</f>
+        <f t="shared" si="8"/>
         <v>5.9868129078691143E-3</v>
       </c>
       <c r="K52" s="11"/>
       <c r="L52">
-        <f>1/J52</f>
+        <f t="shared" si="9"/>
         <v>167.03378164458624</v>
       </c>
       <c r="M52" s="11"/>
       <c r="N52">
-        <f>((H52-G52)/(F52-E52))</f>
+        <f t="shared" si="10"/>
         <v>8.7316054052675573E-8</v>
       </c>
       <c r="O52" s="11"/>
       <c r="P52">
-        <f>1/N52</f>
+        <f t="shared" si="11"/>
         <v>11452647.635642413</v>
       </c>
       <c r="Q52" s="11"/>
       <c r="R52" s="11"/>
       <c r="S52" s="11"/>
-      <c r="T52" s="11"/>
+      <c r="T52" s="13">
+        <f t="shared" si="13"/>
+        <v>13712971.738868138</v>
+      </c>
       <c r="U52" s="11"/>
       <c r="V52" s="11"/>
       <c r="W52" s="10">
@@ -5968,11 +6704,11 @@
       <c r="B53" s="3"/>
       <c r="C53" s="11"/>
       <c r="D53">
-        <f>D52+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.7000000000000004</v>
       </c>
       <c r="E53">
-        <f>D53-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.0080000000000005</v>
       </c>
       <c r="F53">
@@ -5986,28 +6722,31 @@
       </c>
       <c r="I53" s="11"/>
       <c r="J53">
-        <f>((H53-G53)/(F53-E53))/G53</f>
+        <f t="shared" si="8"/>
         <v>5.6731524356411506E-3</v>
       </c>
       <c r="K53" s="11"/>
       <c r="L53">
-        <f>1/J53</f>
+        <f t="shared" si="9"/>
         <v>176.26884018091525</v>
       </c>
       <c r="M53" s="11"/>
       <c r="N53">
-        <f>((H53-G53)/(F53-E53))</f>
+        <f t="shared" si="10"/>
         <v>1.0158484408520958E-7</v>
       </c>
       <c r="O53" s="11"/>
       <c r="P53">
-        <f>1/N53</f>
+        <f t="shared" si="11"/>
         <v>9843988.1362735368</v>
       </c>
       <c r="Q53" s="11"/>
       <c r="R53" s="11"/>
       <c r="S53" s="11"/>
-      <c r="T53" s="11"/>
+      <c r="T53" s="13">
+        <f t="shared" si="13"/>
+        <v>11169289.054344561</v>
+      </c>
       <c r="U53" s="11"/>
       <c r="V53" s="11"/>
       <c r="W53" s="10">
@@ -6023,11 +6762,11 @@
       <c r="B54" s="3"/>
       <c r="C54" s="11"/>
       <c r="D54">
-        <f>D53+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.8000000000000005</v>
       </c>
       <c r="E54">
-        <f>D54-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.1080000000000005</v>
       </c>
       <c r="F54">
@@ -6041,28 +6780,31 @@
       </c>
       <c r="I54" s="11"/>
       <c r="J54">
-        <f>((H54-G54)/(F54-E54))/G54</f>
+        <f t="shared" si="8"/>
         <v>5.3231121120673065E-3</v>
       </c>
       <c r="K54" s="11"/>
       <c r="L54">
-        <f>1/J54</f>
+        <f t="shared" si="9"/>
         <v>187.86002979967967</v>
       </c>
       <c r="M54" s="11"/>
       <c r="N54">
-        <f>((H54-G54)/(F54-E54))</f>
+        <f t="shared" si="10"/>
         <v>1.1450671068271107E-7</v>
       </c>
       <c r="O54" s="11"/>
       <c r="P54">
-        <f>1/N54</f>
+        <f t="shared" si="11"/>
         <v>8733112.6187959407</v>
       </c>
       <c r="Q54" s="11"/>
       <c r="R54" s="11"/>
       <c r="S54" s="11"/>
-      <c r="T54" s="11"/>
+      <c r="T54" s="13">
+        <f t="shared" si="13"/>
+        <v>9297467.511432102</v>
+      </c>
       <c r="U54" s="11"/>
       <c r="V54" s="11"/>
       <c r="W54" s="10">
@@ -6078,11 +6820,11 @@
       <c r="B55" s="3"/>
       <c r="C55" s="11"/>
       <c r="D55">
-        <f>D54+0.1</f>
+        <f t="shared" si="12"/>
         <v>1.9000000000000006</v>
       </c>
       <c r="E55">
-        <f>D55-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.2080000000000006</v>
       </c>
       <c r="F55">
@@ -6096,28 +6838,31 @@
       </c>
       <c r="I55" s="11"/>
       <c r="J55">
-        <f>((H55-G55)/(F55-E55))/G55</f>
+        <f t="shared" si="8"/>
         <v>-0.96095256033080201</v>
       </c>
       <c r="K55" s="11"/>
       <c r="L55">
-        <f>1/J55</f>
+        <f t="shared" si="9"/>
         <v>-1.0406340971252068</v>
       </c>
       <c r="M55" s="11"/>
       <c r="N55">
-        <f>((H55-G55)/(F55-E55))</f>
+        <f t="shared" si="10"/>
         <v>-2.4394086050915834E-5</v>
       </c>
       <c r="O55" s="11"/>
       <c r="P55">
-        <f>1/N55</f>
+        <f t="shared" si="11"/>
         <v>-40993.542365669273</v>
       </c>
       <c r="Q55" s="11"/>
       <c r="R55" s="11"/>
       <c r="S55" s="11"/>
-      <c r="T55" s="11"/>
+      <c r="T55" s="13">
+        <f t="shared" si="13"/>
+        <v>7878569.898663817</v>
+      </c>
       <c r="U55" s="11"/>
       <c r="V55" s="11"/>
       <c r="W55" s="10">
@@ -6133,11 +6878,11 @@
       <c r="B56" s="3"/>
       <c r="C56" s="11"/>
       <c r="D56">
-        <f>D55+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.0000000000000004</v>
       </c>
       <c r="E56">
-        <f>D56-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.3080000000000005</v>
       </c>
       <c r="F56">
@@ -6151,28 +6896,31 @@
       </c>
       <c r="I56" s="11"/>
       <c r="J56">
-        <f>((H56-G56)/(F56-E56))/G56</f>
+        <f t="shared" si="8"/>
         <v>4.4844700737728047E-3</v>
       </c>
       <c r="K56" s="11"/>
       <c r="L56">
-        <f>1/J56</f>
+        <f t="shared" si="9"/>
         <v>222.99178800377086</v>
       </c>
       <c r="M56" s="11"/>
       <c r="N56">
-        <f>((H56-G56)/(F56-E56))</f>
+        <f t="shared" si="10"/>
         <v>1.3235704723212944E-7</v>
       </c>
       <c r="O56" s="11"/>
       <c r="P56">
-        <f>1/N56</f>
+        <f t="shared" si="11"/>
         <v>7555321.162810375</v>
       </c>
       <c r="Q56" s="11"/>
       <c r="R56" s="11"/>
       <c r="S56" s="11"/>
-      <c r="T56" s="11"/>
+      <c r="T56" s="13">
+        <f t="shared" si="13"/>
+        <v>6776322.3304730952</v>
+      </c>
       <c r="U56" s="11"/>
       <c r="V56" s="11"/>
       <c r="W56" s="10">
@@ -6188,11 +6936,11 @@
       <c r="B57" s="3"/>
       <c r="C57" s="11"/>
       <c r="D57">
-        <f>D56+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.1000000000000005</v>
       </c>
       <c r="E57">
-        <f>D57-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.4080000000000006</v>
       </c>
       <c r="F57">
@@ -6206,28 +6954,31 @@
       </c>
       <c r="I57" s="11"/>
       <c r="J57">
-        <f>((H57-G57)/(F57-E57))/G57</f>
+        <f t="shared" si="8"/>
         <v>3.9779880847574198E-3</v>
       </c>
       <c r="K57" s="11"/>
       <c r="L57">
-        <f>1/J57</f>
+        <f t="shared" si="9"/>
         <v>251.38335728850745</v>
       </c>
       <c r="M57" s="11"/>
       <c r="N57">
-        <f>((H57-G57)/(F57-E57))</f>
+        <f t="shared" si="10"/>
         <v>1.3479557521860711E-7</v>
       </c>
       <c r="O57" s="11"/>
       <c r="P57">
-        <f>1/N57</f>
+        <f t="shared" si="11"/>
         <v>7418641.1414338509</v>
       </c>
       <c r="Q57" s="11"/>
       <c r="R57" s="11"/>
       <c r="S57" s="11"/>
-      <c r="T57" s="11"/>
+      <c r="T57" s="13">
+        <f t="shared" si="13"/>
+        <v>5902253.2131430088</v>
+      </c>
       <c r="U57" s="11"/>
       <c r="V57" s="11"/>
       <c r="W57" s="10">
@@ -6243,11 +6994,11 @@
       <c r="B58" s="3"/>
       <c r="C58" s="11"/>
       <c r="D58">
-        <f>D57+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.2000000000000006</v>
       </c>
       <c r="E58">
-        <f>D58-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.5080000000000007</v>
       </c>
       <c r="F58">
@@ -6261,28 +7012,31 @@
       </c>
       <c r="I58" s="11"/>
       <c r="J58">
-        <f>((H58-G58)/(F58-E58))/G58</f>
+        <f t="shared" si="8"/>
         <v>3.3985595571676191E-3</v>
       </c>
       <c r="K58" s="11"/>
       <c r="L58">
-        <f>1/J58</f>
+        <f t="shared" si="9"/>
         <v>294.24230565298853</v>
       </c>
       <c r="M58" s="11"/>
       <c r="N58">
-        <f>((H58-G58)/(F58-E58))</f>
+        <f t="shared" si="10"/>
         <v>1.3079264655451873E-7</v>
       </c>
       <c r="O58" s="11"/>
       <c r="P58">
-        <f>1/N58</f>
+        <f t="shared" si="11"/>
         <v>7645689.771887647</v>
       </c>
       <c r="Q58" s="11"/>
       <c r="R58" s="11"/>
       <c r="S58" s="11"/>
-      <c r="T58" s="11"/>
+      <c r="T58" s="13">
+        <f t="shared" si="13"/>
+        <v>5196866.4090774953</v>
+      </c>
       <c r="U58" s="11"/>
       <c r="V58" s="11"/>
       <c r="W58" s="10">
@@ -6298,11 +7052,11 @@
       <c r="B59" s="3"/>
       <c r="C59" s="11"/>
       <c r="D59">
-        <f>D58+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.3000000000000007</v>
       </c>
       <c r="E59">
-        <f>D59-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.6080000000000008</v>
       </c>
       <c r="F59">
@@ -6316,28 +7070,31 @@
       </c>
       <c r="I59" s="11"/>
       <c r="J59">
-        <f>((H59-G59)/(F59-E59))/G59</f>
+        <f t="shared" si="8"/>
         <v>2.7316264984510409E-3</v>
       </c>
       <c r="K59" s="11"/>
       <c r="L59">
-        <f>1/J59</f>
+        <f t="shared" si="9"/>
         <v>366.08225925727635</v>
       </c>
       <c r="M59" s="11"/>
       <c r="N59">
-        <f>((H59-G59)/(F59-E59))</f>
+        <f t="shared" si="10"/>
         <v>1.1827946344970568E-7</v>
       </c>
       <c r="O59" s="11"/>
       <c r="P59">
-        <f>1/N59</f>
+        <f t="shared" si="11"/>
         <v>8454553.0630109422</v>
       </c>
       <c r="Q59" s="11"/>
       <c r="R59" s="11"/>
       <c r="S59" s="11"/>
-      <c r="T59" s="11"/>
+      <c r="T59" s="13">
+        <f t="shared" si="13"/>
+        <v>4618936.2358962204</v>
+      </c>
       <c r="U59" s="11"/>
       <c r="V59" s="11"/>
       <c r="W59" s="10">
@@ -6353,11 +7110,11 @@
       <c r="B60" s="3"/>
       <c r="C60" s="11"/>
       <c r="D60">
-        <f>D59+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.4000000000000008</v>
       </c>
       <c r="E60">
-        <f>D60-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.7080000000000009</v>
       </c>
       <c r="F60">
@@ -6371,28 +7128,31 @@
       </c>
       <c r="I60" s="11"/>
       <c r="J60">
-        <f>((H60-G60)/(F60-E60))/G60</f>
+        <f t="shared" si="8"/>
         <v>1.9592155065743756E-3</v>
       </c>
       <c r="K60" s="11"/>
       <c r="L60">
-        <f>1/J60</f>
+        <f t="shared" si="9"/>
         <v>510.40837347621209</v>
       </c>
       <c r="M60" s="11"/>
       <c r="N60">
-        <f>((H60-G60)/(F60-E60))</f>
+        <f t="shared" si="10"/>
         <v>9.466742967424326E-8</v>
       </c>
       <c r="O60" s="11"/>
       <c r="P60">
-        <f>1/N60</f>
+        <f t="shared" si="11"/>
         <v>10563295.142173655</v>
       </c>
       <c r="Q60" s="11"/>
       <c r="R60" s="11"/>
       <c r="S60" s="11"/>
-      <c r="T60" s="11"/>
+      <c r="T60" s="13">
+        <f t="shared" si="13"/>
+        <v>4139154.3286136794</v>
+      </c>
       <c r="U60" s="11"/>
       <c r="V60" s="11"/>
       <c r="W60" s="10">
@@ -6408,11 +7168,11 @@
       <c r="B61" s="3"/>
       <c r="C61" s="11"/>
       <c r="D61">
-        <f>D60+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.5000000000000009</v>
       </c>
       <c r="E61">
-        <f>D61-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.8080000000000009</v>
       </c>
       <c r="F61">
@@ -6426,28 +7186,31 @@
       </c>
       <c r="I61" s="11"/>
       <c r="J61">
-        <f>((H61-G61)/(F61-E61))/G61</f>
+        <f t="shared" si="8"/>
         <v>1.0585025575981738E-3</v>
       </c>
       <c r="K61" s="11"/>
       <c r="L61">
-        <f>1/J61</f>
+        <f t="shared" si="9"/>
         <v>944.73083019192632</v>
       </c>
       <c r="M61" s="11"/>
       <c r="N61">
-        <f>((H61-G61)/(F61-E61))</f>
+        <f t="shared" si="10"/>
         <v>5.6661763752813193E-8</v>
       </c>
       <c r="O61" s="11"/>
       <c r="P61">
-        <f>1/N61</f>
+        <f t="shared" si="11"/>
         <v>17648585.814633261</v>
       </c>
       <c r="Q61" s="11"/>
       <c r="R61" s="11"/>
       <c r="S61" s="11"/>
-      <c r="T61" s="11"/>
+      <c r="T61" s="13">
+        <f t="shared" si="13"/>
+        <v>3736214.6445560316</v>
+      </c>
       <c r="U61" s="11"/>
       <c r="V61" s="11"/>
       <c r="W61" s="10">
@@ -6463,11 +7226,11 @@
       <c r="B62" s="3"/>
       <c r="C62" s="11"/>
       <c r="D62">
-        <f>D61+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.600000000000001</v>
       </c>
       <c r="E62">
-        <f>D62-0.692</f>
+        <f t="shared" si="7"/>
         <v>1.908000000000001</v>
       </c>
       <c r="F62">
@@ -6481,28 +7244,31 @@
       </c>
       <c r="I62" s="11"/>
       <c r="J62">
-        <f>((H62-G62)/(F62-E62))/G62</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K62" s="11"/>
       <c r="L62" t="e">
-        <f>1/J62</f>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M62" s="11"/>
       <c r="N62">
-        <f>((H62-G62)/(F62-E62))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O62" s="11"/>
       <c r="P62" t="e">
-        <f>1/N62</f>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q62" s="11"/>
       <c r="R62" s="11"/>
       <c r="S62" s="11"/>
-      <c r="T62" s="11"/>
+      <c r="T62" s="13">
+        <f t="shared" si="13"/>
+        <v>3394320.4335990897</v>
+      </c>
       <c r="U62" s="11"/>
       <c r="V62" s="11"/>
       <c r="W62" s="10">
@@ -6518,11 +7284,11 @@
       <c r="B63" s="3"/>
       <c r="C63" s="11"/>
       <c r="D63">
-        <f>D62+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.7000000000000011</v>
       </c>
       <c r="E63">
-        <f>D63-0.692</f>
+        <f t="shared" si="7"/>
         <v>2.0080000000000009</v>
       </c>
       <c r="F63">
@@ -6536,28 +7302,31 @@
       </c>
       <c r="I63" s="11"/>
       <c r="J63">
-        <f>((H63-G63)/(F63-E63))/G63</f>
+        <f t="shared" si="8"/>
         <v>-1.2549722853438484E-3</v>
       </c>
       <c r="K63" s="11"/>
       <c r="L63">
-        <f>1/J63</f>
+        <f t="shared" si="9"/>
         <v>-796.83034572035285</v>
       </c>
       <c r="M63" s="11"/>
       <c r="N63">
-        <f>((H63-G63)/(F63-E63))</f>
+        <f t="shared" si="10"/>
         <v>-8.0925318046286665E-8</v>
       </c>
       <c r="O63" s="11"/>
       <c r="P63">
-        <f>1/N63</f>
+        <f t="shared" si="11"/>
         <v>-12357072.225876609</v>
       </c>
       <c r="Q63" s="11"/>
       <c r="R63" s="11"/>
       <c r="S63" s="11"/>
-      <c r="T63" s="11"/>
+      <c r="T63" s="13">
+        <f t="shared" si="13"/>
+        <v>3101556.6342934729</v>
+      </c>
       <c r="U63" s="11"/>
       <c r="V63" s="11"/>
       <c r="W63" s="10">
@@ -6573,11 +7342,11 @@
       <c r="B64" s="3"/>
       <c r="C64" s="11"/>
       <c r="D64">
-        <f>D63+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.8000000000000012</v>
       </c>
       <c r="E64">
-        <f>D64-0.692</f>
+        <f t="shared" si="7"/>
         <v>2.1080000000000014</v>
       </c>
       <c r="F64">
@@ -6591,28 +7360,31 @@
       </c>
       <c r="I64" s="11"/>
       <c r="J64">
-        <f>((H64-G64)/(F64-E64))/G64</f>
+        <f t="shared" si="8"/>
         <v>-2.7579856291872866E-3</v>
       </c>
       <c r="K64" s="11"/>
       <c r="L64">
-        <f>1/J64</f>
+        <f t="shared" si="9"/>
         <v>-362.58347013021836</v>
       </c>
       <c r="M64" s="11"/>
       <c r="N64">
-        <f>((H64-G64)/(F64-E64))</f>
+        <f t="shared" si="10"/>
         <v>-1.9362470761702955E-7</v>
       </c>
       <c r="O64" s="11"/>
       <c r="P64">
-        <f>1/N64</f>
+        <f t="shared" si="11"/>
         <v>-5164630.1358290529</v>
       </c>
       <c r="Q64" s="11"/>
       <c r="R64" s="11"/>
       <c r="S64" s="11"/>
-      <c r="T64" s="11"/>
+      <c r="T64" s="13">
+        <f t="shared" si="13"/>
+        <v>2848795.1389368223</v>
+      </c>
       <c r="U64" s="11"/>
       <c r="V64" s="11"/>
       <c r="W64" s="10">
@@ -6628,11 +7400,11 @@
       <c r="B65" s="3"/>
       <c r="C65" s="11"/>
       <c r="D65">
-        <f>D64+0.1</f>
+        <f t="shared" si="12"/>
         <v>2.9000000000000012</v>
       </c>
       <c r="E65">
-        <f>D65-0.692</f>
+        <f t="shared" si="7"/>
         <v>2.2080000000000011</v>
       </c>
       <c r="F65">
@@ -6646,28 +7418,31 @@
       </c>
       <c r="I65" s="11"/>
       <c r="J65">
-        <f>((H65-G65)/(F65-E65))/G65</f>
+        <f t="shared" si="8"/>
         <v>-4.5798835219698969E-3</v>
       </c>
       <c r="K65" s="11"/>
       <c r="L65">
-        <f>1/J65</f>
+        <f t="shared" si="9"/>
         <v>-218.34616430810027</v>
       </c>
       <c r="M65" s="11"/>
       <c r="N65">
-        <f>((H65-G65)/(F65-E65))</f>
+        <f t="shared" si="10"/>
         <v>-3.4841975783965864E-7</v>
       </c>
       <c r="O65" s="11"/>
       <c r="P65">
-        <f>1/N65</f>
+        <f t="shared" si="11"/>
         <v>-2870101.3002259075</v>
       </c>
       <c r="Q65" s="11"/>
       <c r="R65" s="11"/>
       <c r="S65" s="11"/>
-      <c r="T65" s="11"/>
+      <c r="T65" s="13">
+        <f t="shared" si="13"/>
+        <v>2628945.9302578019</v>
+      </c>
       <c r="U65" s="11"/>
       <c r="V65" s="11"/>
       <c r="W65" s="10">
@@ -6683,11 +7458,11 @@
       <c r="B66" s="3"/>
       <c r="C66" s="11"/>
       <c r="D66">
-        <f>D65+0.1</f>
+        <f t="shared" si="12"/>
         <v>3.0000000000000013</v>
       </c>
       <c r="E66">
-        <f>D66-0.692</f>
+        <f t="shared" si="7"/>
         <v>2.3080000000000016</v>
       </c>
       <c r="F66">
@@ -6701,28 +7476,31 @@
       </c>
       <c r="I66" s="11"/>
       <c r="J66">
-        <f>((H66-G66)/(F66-E66))/G66</f>
+        <f t="shared" si="8"/>
         <v>-6.8200370065315558E-3</v>
       </c>
       <c r="K66" s="11"/>
       <c r="L66">
-        <f>1/J66</f>
+        <f t="shared" si="9"/>
         <v>-146.62677035950085</v>
       </c>
       <c r="M66" s="11"/>
       <c r="N66">
-        <f>((H66-G66)/(F66-E66))</f>
+        <f t="shared" si="10"/>
         <v>-5.5983799674938868E-7</v>
       </c>
       <c r="O66" s="11"/>
       <c r="P66">
-        <f>1/N66</f>
+        <f t="shared" si="11"/>
         <v>-1786231.0272013382</v>
       </c>
       <c r="Q66" s="11"/>
       <c r="R66" s="11"/>
       <c r="S66" s="11"/>
-      <c r="T66" s="11"/>
+      <c r="T66" s="13">
+        <f t="shared" si="13"/>
+        <v>2436432.3415456</v>
+      </c>
       <c r="U66" s="11"/>
       <c r="V66" s="11"/>
       <c r="W66" s="10">
@@ -6738,11 +7516,11 @@
       <c r="B67" s="3"/>
       <c r="C67" s="11"/>
       <c r="D67">
-        <f>D66+0.1</f>
+        <f t="shared" si="12"/>
         <v>3.1000000000000014</v>
       </c>
       <c r="E67">
-        <f>D67-0.692</f>
+        <f t="shared" si="7"/>
         <v>2.4080000000000013</v>
       </c>
       <c r="F67">
@@ -6756,28 +7534,31 @@
       </c>
       <c r="I67" s="11"/>
       <c r="J67">
-        <f>((H67-G67)/(F67-E67))/G67</f>
+        <f t="shared" si="8"/>
         <v>-2.2325297856498736</v>
       </c>
       <c r="K67" s="11"/>
       <c r="L67">
-        <f>1/J67</f>
+        <f t="shared" si="9"/>
         <v>-0.44792235536015795</v>
       </c>
       <c r="M67" s="11"/>
       <c r="N67">
-        <f>((H67-G67)/(F67-E67))</f>
+        <f t="shared" si="10"/>
         <v>-1.9697470821736771E-4</v>
       </c>
       <c r="O67" s="11"/>
       <c r="P67">
-        <f>1/N67</f>
+        <f t="shared" si="11"/>
         <v>-5076.7939145591672</v>
       </c>
       <c r="Q67" s="11"/>
       <c r="R67" s="11"/>
       <c r="S67" s="11"/>
-      <c r="T67" s="11"/>
+      <c r="T67" s="13">
+        <f t="shared" si="13"/>
+        <v>2266818.725971872</v>
+      </c>
       <c r="U67" s="11"/>
       <c r="V67" s="11"/>
       <c r="W67" s="10">
@@ -6793,11 +7574,11 @@
       <c r="B68" s="3"/>
       <c r="C68" s="11"/>
       <c r="D68">
-        <f>D67+0.1</f>
+        <f t="shared" si="12"/>
         <v>3.2000000000000015</v>
       </c>
       <c r="E68">
-        <f>D68-0.692</f>
+        <f t="shared" si="7"/>
         <v>2.5080000000000018</v>
       </c>
       <c r="F68">
@@ -6811,28 +7592,31 @@
       </c>
       <c r="I68" s="11"/>
       <c r="J68">
-        <f>((H68-G68)/(F68-E68))/G68</f>
+        <f t="shared" si="8"/>
         <v>-1.3205085288349006E-2</v>
       </c>
       <c r="K68" s="11"/>
       <c r="L68">
-        <f>1/J68</f>
+        <f t="shared" si="9"/>
         <v>-75.728401457755908</v>
       </c>
       <c r="M68" s="11"/>
       <c r="N68">
-        <f>((H68-G68)/(F68-E68))</f>
+        <f t="shared" si="10"/>
         <v>-1.2477991703869866E-6</v>
       </c>
       <c r="O68" s="11"/>
       <c r="P68">
-        <f>1/N68</f>
+        <f t="shared" si="11"/>
         <v>-801411.01527569105</v>
       </c>
       <c r="Q68" s="11"/>
       <c r="R68" s="11"/>
       <c r="S68" s="11"/>
-      <c r="T68" s="11"/>
+      <c r="T68" s="13">
+        <f t="shared" si="13"/>
+        <v>2116540.1615475737</v>
+      </c>
       <c r="U68" s="11"/>
       <c r="V68" s="11"/>
       <c r="W68" s="10">
@@ -6848,11 +7632,11 @@
       <c r="B69" s="3"/>
       <c r="C69" s="11"/>
       <c r="D69">
-        <f>D68+0.1</f>
+        <f t="shared" si="12"/>
         <v>3.3000000000000016</v>
       </c>
       <c r="E69">
-        <f>D69-0.692</f>
+        <f t="shared" si="7"/>
         <v>2.6080000000000014</v>
       </c>
       <c r="F69">
@@ -6866,28 +7650,31 @@
       </c>
       <c r="I69" s="11"/>
       <c r="J69">
-        <f>((H69-G69)/(F69-E69))/G69</f>
+        <f t="shared" si="8"/>
         <v>-1.7910427964701388E-2</v>
       </c>
       <c r="K69" s="11"/>
       <c r="L69">
-        <f>1/J69</f>
+        <f t="shared" si="9"/>
         <v>-55.833395046217845</v>
       </c>
       <c r="M69" s="11"/>
       <c r="N69">
-        <f>((H69-G69)/(F69-E69))</f>
+        <f t="shared" si="10"/>
         <v>-1.806666538915765E-6</v>
       </c>
       <c r="O69" s="11"/>
       <c r="P69">
-        <f>1/N69</f>
+        <f t="shared" si="11"/>
         <v>-553505.57419418974</v>
       </c>
       <c r="Q69" s="11"/>
       <c r="R69" s="11"/>
       <c r="S69" s="11"/>
-      <c r="T69" s="11"/>
+      <c r="T69" s="13">
+        <f t="shared" si="13"/>
+        <v>1982704.342933143</v>
+      </c>
       <c r="U69" s="11"/>
       <c r="V69" s="11"/>
       <c r="W69" s="10">
@@ -7131,6 +7918,90 @@
       <c r="Y77" s="11"/>
       <c r="Z77" s="11"/>
     </row>
+    <row r="85" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H85" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I85" s="6"/>
+    </row>
+    <row r="86" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H86" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I86" s="6"/>
+    </row>
+    <row r="87" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M87" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N87" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M88" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N88" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="89" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>48</v>
+      </c>
+      <c r="E89">
+        <v>1.25</v>
+      </c>
+      <c r="G89">
+        <v>32179928.559999999</v>
+      </c>
+      <c r="H89">
+        <v>24914183</v>
+      </c>
+      <c r="I89">
+        <f>(G89*H89)/(G89+H89)</f>
+        <v>14042369.820015928</v>
+      </c>
+      <c r="K89">
+        <f>-2*POWER(10,-5)</f>
+        <v>-2.0000000000000002E-5</v>
+      </c>
+      <c r="M89">
+        <f>K89*I89</f>
+        <v>-280.84739640031859</v>
+      </c>
+      <c r="N89">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="90" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>49</v>
+      </c>
+      <c r="E90">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="93" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
calcolo delle tensioni di modo comune
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD9CE9A-4586-407C-AB44-DADF087BA270}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0702B8B-7B52-479F-9B87-3B5F83371AD1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="118">
   <si>
     <t>Ib</t>
   </si>
@@ -220,9 +220,6 @@
     <t>IdMB (teo)</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>P_hp</t>
   </si>
   <si>
@@ -320,6 +317,75 @@
   </si>
   <si>
     <t>GVO_risultante</t>
+  </si>
+  <si>
+    <t>Vcm=0,5</t>
+  </si>
+  <si>
+    <t>Add_stima</t>
+  </si>
+  <si>
+    <t>Vds &lt; Vgs - Vth</t>
+  </si>
+  <si>
+    <t>Vd - Vs &lt; Vg - Vs - Vth</t>
+  </si>
+  <si>
+    <t>Vd &lt; Vg - Vth</t>
+  </si>
+  <si>
+    <t>Vg &gt; Vd + Vth</t>
+  </si>
+  <si>
+    <t>Condizione per avere saturazione</t>
+  </si>
+  <si>
+    <t>Scompongo i termini nei potenziali</t>
+  </si>
+  <si>
+    <t>Risolvo</t>
+  </si>
+  <si>
+    <t>Sostituisco con i termini del circuito</t>
+  </si>
+  <si>
+    <t>Vds_3 = Vgs_3 = GVO_3 + Vth_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vcm_min &gt; GVO_3 + Vth_3 + Vth_1 </t>
+  </si>
+  <si>
+    <t>Vcm_min</t>
+  </si>
+  <si>
+    <t>Calcolo Vcm e Dinamica (PMOS)</t>
+  </si>
+  <si>
+    <t>Vcm_max</t>
+  </si>
+  <si>
+    <t>Vdd + Vds_5 + Vgs_1 - Vcm = 0</t>
+  </si>
+  <si>
+    <t>Vds_5 &lt; GVO_5</t>
+  </si>
+  <si>
+    <t>Vgs1 = GVO_1 + Vth_1</t>
+  </si>
+  <si>
+    <t>Io ho queste 3 condizioni</t>
+  </si>
+  <si>
+    <t>Vds_5 = Vcm - Vgs_1 - Vdd</t>
+  </si>
+  <si>
+    <t>Vcm - Vgs_1 - Vdd &lt; GVO_5</t>
+  </si>
+  <si>
+    <t>Risolvendo ottengo</t>
+  </si>
+  <si>
+    <t>Vcm_max &lt; Vdd + GVO_5 + GVO_1 + Vth_1</t>
   </si>
 </sst>
 </file>
@@ -368,7 +434,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +453,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -400,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -419,6 +491,10 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2946,10 +3022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q183"/>
+  <dimension ref="B2:AH183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,7 +3036,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
     <col min="14" max="14" width="21.140625" customWidth="1"/>
-    <col min="16" max="16" width="28.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
     <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3195,13 +3271,7 @@
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21">
-        <f>(G16+G12+G10+C6)*C4</f>
-        <v>5.8409999999999998E-5</v>
-      </c>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="N22" s="2" t="s">
@@ -3210,7 +3280,7 @@
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="14">
         <v>30</v>
@@ -3222,7 +3292,7 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="14">
         <v>20000</v>
@@ -3273,7 +3343,7 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="14">
         <v>10</v>
@@ -3297,7 +3367,7 @@
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="14">
         <v>20</v>
@@ -3318,7 +3388,7 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="14">
         <v>20</v>
@@ -3355,14 +3425,14 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="14">
         <f>(C27+C28+C26)*C25</f>
         <v>165</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M30">
         <v>30</v>
@@ -3383,14 +3453,14 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C31">
         <f>C23/SQRT(C24)</f>
         <v>0.21213203435596426</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J31" s="2"/>
       <c r="M31">
@@ -3413,53 +3483,92 @@
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L33" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34">
         <v>0.15</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L34" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="16"/>
+      <c r="Y34" s="16"/>
+      <c r="Z34" s="16"/>
+      <c r="AA34" s="16"/>
+      <c r="AB34" s="16"/>
+      <c r="AC34" s="16"/>
+      <c r="AD34" s="16"/>
+      <c r="AE34" s="16"/>
+      <c r="AF34" s="16"/>
+      <c r="AG34" s="16"/>
+      <c r="AH34" s="16"/>
+    </row>
+    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="H35" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I35" s="15"/>
       <c r="J35" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K35" s="15"/>
       <c r="L35" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N35" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O35" s="15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R35" s="16"/>
+      <c r="S35" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="16"/>
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="16"/>
+      <c r="AH35" s="16"/>
+    </row>
+    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36">
         <f>C26</f>
         <v>10</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F36">
         <f>2*C36*POWER(10,-6)/($C$14*$C$34*$C$34)</f>
@@ -3470,73 +3579,111 @@
         <v>14</v>
       </c>
       <c r="J36">
-        <f>1.4*H36</f>
+        <f t="shared" ref="J36:J43" si="2">1.4*H36</f>
         <v>19.599999999999998</v>
       </c>
       <c r="L36">
         <v>10</v>
       </c>
       <c r="N36">
-        <v>0.185</v>
+        <v>-0.185</v>
       </c>
       <c r="O36">
         <v>-0.877</v>
       </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="16"/>
+      <c r="Z36" s="16"/>
+      <c r="AA36" s="16"/>
+      <c r="AB36" s="16"/>
+      <c r="AC36" s="16"/>
+      <c r="AD36" s="16"/>
+      <c r="AE36" s="16"/>
+      <c r="AF36" s="16"/>
+      <c r="AG36" s="16"/>
+      <c r="AH36" s="16"/>
+    </row>
+    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C37">
         <f>C27</f>
         <v>20</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F37">
-        <f t="shared" ref="F37:F43" si="2">2*C37*POWER(10,-6)/($C$14*$C$34*$C$34)</f>
+        <f t="shared" ref="F37:F41" si="3">2*C37*POWER(10,-6)/($C$14*$C$34*$C$34)</f>
         <v>26.993285420251706</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37:H43" si="3">ROUNDUP(F37,0)</f>
+        <f t="shared" ref="H37:H43" si="4">ROUNDUP(F37,0)</f>
         <v>27</v>
       </c>
       <c r="J37">
-        <f>1.4*H37</f>
+        <f t="shared" si="2"/>
         <v>37.799999999999997</v>
       </c>
       <c r="L37">
         <v>20.350000000000001</v>
       </c>
       <c r="N37">
-        <v>0.185</v>
+        <v>-0.185</v>
       </c>
       <c r="O37">
         <v>-0.877</v>
       </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R37" s="16"/>
+      <c r="S37" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="16"/>
+      <c r="Y37" s="16"/>
+      <c r="Z37" s="16"/>
+      <c r="AA37" s="16"/>
+      <c r="AB37" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC37" s="16"/>
+      <c r="AD37" s="16"/>
+      <c r="AE37" s="16"/>
+      <c r="AF37" s="16"/>
+      <c r="AG37" s="16"/>
+      <c r="AH37" s="16"/>
+    </row>
+    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38">
         <f>C27/2</f>
         <v>10</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F38">
         <f>2*C38*POWER(10,-6)/($C$16*$C$34*$C$34)</f>
         <v>4.0952053335954268</v>
       </c>
       <c r="H38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="J38">
-        <f>1.4*H38</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L38">
@@ -3548,28 +3695,45 @@
       <c r="O38">
         <v>0.68500000000000005</v>
       </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
+      <c r="Y38" s="16"/>
+      <c r="Z38" s="16"/>
+      <c r="AA38" s="16"/>
+      <c r="AB38" s="16"/>
+      <c r="AC38" s="16"/>
+      <c r="AD38" s="16"/>
+      <c r="AE38" s="16"/>
+      <c r="AF38" s="16"/>
+      <c r="AG38" s="16"/>
+      <c r="AH38" s="16"/>
+    </row>
+    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39">
         <f>C27/2</f>
         <v>10</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F39">
         <f>2*C39*POWER(10,-6)/($C$16*$C$34*$C$34)</f>
         <v>4.0952053335954268</v>
       </c>
       <c r="H39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="J39">
-        <f>1.4*H39</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L39">
@@ -3581,84 +3745,161 @@
       <c r="O39">
         <v>0.68500000000000005</v>
       </c>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R39" s="16"/>
+      <c r="S39" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="16"/>
+      <c r="AB39" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC39" s="16"/>
+      <c r="AD39" s="16"/>
+      <c r="AE39" s="16"/>
+      <c r="AF39" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="16"/>
+    </row>
+    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40">
         <f>C27/2</f>
         <v>10</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F40">
+        <f t="shared" si="3"/>
+        <v>13.496642710125853</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="J40">
         <f t="shared" si="2"/>
-        <v>13.496642710125853</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="J40">
-        <f>1.4*H40</f>
         <v>19.599999999999998</v>
       </c>
       <c r="L40">
         <v>10.18</v>
       </c>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>-0.186</v>
+      </c>
+      <c r="O40">
+        <v>-0.878</v>
+      </c>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="16"/>
+      <c r="Y40" s="16"/>
+      <c r="Z40" s="16"/>
+      <c r="AA40" s="16"/>
+      <c r="AB40" s="16"/>
+      <c r="AC40" s="16"/>
+      <c r="AD40" s="16"/>
+      <c r="AE40" s="16"/>
+      <c r="AF40" s="16"/>
+      <c r="AG40" s="16"/>
+      <c r="AH40" s="16"/>
+    </row>
+    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41">
         <f>C27/2</f>
         <v>10</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41">
+        <f t="shared" si="3"/>
+        <v>13.496642710125853</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="J41">
         <f t="shared" si="2"/>
-        <v>13.496642710125853</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="J41">
-        <f>1.4*H41</f>
         <v>19.599999999999998</v>
       </c>
       <c r="L41">
         <v>10.18</v>
       </c>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>-0.186</v>
+      </c>
+      <c r="O41">
+        <v>-0.878</v>
+      </c>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="X41" s="16"/>
+      <c r="Y41" s="16"/>
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC41" s="16"/>
+      <c r="AD41" s="16"/>
+      <c r="AE41" s="16"/>
+      <c r="AF41" s="16"/>
+      <c r="AG41" s="16"/>
+      <c r="AH41" s="16"/>
+    </row>
+    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42">
         <f>C28</f>
         <v>20</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F42">
         <f>2*C42*POWER(10,-6)/($C$16*$C$34*$C$34)</f>
         <v>8.1904106671908536</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H42">
         <v>10</v>
       </c>
       <c r="J42">
-        <f>1.4*H42</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="L42">
@@ -3670,94 +3911,367 @@
       <c r="O42">
         <v>0.68500000000000005</v>
       </c>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="16"/>
+      <c r="Y42" s="16"/>
+      <c r="Z42" s="16"/>
+      <c r="AA42" s="16"/>
+      <c r="AB42" s="16"/>
+      <c r="AC42" s="16"/>
+      <c r="AD42" s="16"/>
+      <c r="AE42" s="16"/>
+      <c r="AF42" s="16"/>
+      <c r="AG42" s="16"/>
+      <c r="AH42" s="16"/>
+    </row>
+    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43">
         <f>C28</f>
         <v>20</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F43">
         <f>2*C43*POWER(10,-6)/($C$14*$C$34*$C$34)</f>
         <v>26.993285420251706</v>
       </c>
       <c r="H43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
       <c r="J43">
-        <f>1.4*H43</f>
+        <f t="shared" si="2"/>
         <v>37.799999999999997</v>
       </c>
       <c r="L43">
         <v>20.43</v>
       </c>
       <c r="N43">
-        <v>0.185</v>
+        <v>-0.185</v>
       </c>
       <c r="O43">
         <v>-0.877</v>
       </c>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R43" s="16"/>
+      <c r="S43" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC43" s="16"/>
+      <c r="AD43" s="16"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="16"/>
+      <c r="AH43" s="16"/>
+    </row>
+    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="16"/>
+      <c r="Y44" s="16"/>
+      <c r="Z44" s="16"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="16"/>
+      <c r="AC44" s="16"/>
+      <c r="AD44" s="16"/>
+      <c r="AE44" s="16"/>
+      <c r="AF44" s="16"/>
+      <c r="AG44" s="16"/>
+      <c r="AH44" s="16"/>
+    </row>
+    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="R45" s="16"/>
+      <c r="S45" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="16"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="16"/>
+      <c r="Y45" s="16"/>
+      <c r="Z45" s="16"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC45" s="16"/>
+      <c r="AD45" s="16"/>
+      <c r="AE45" s="16"/>
+      <c r="AF45" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG45" s="16"/>
+      <c r="AH45" s="16"/>
+    </row>
+    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="16"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="16"/>
+      <c r="Y46" s="16"/>
+      <c r="Z46" s="16"/>
+      <c r="AA46" s="16"/>
+      <c r="AB46" s="16"/>
+      <c r="AC46" s="16"/>
+      <c r="AD46" s="16"/>
+      <c r="AE46" s="16"/>
+      <c r="AF46" s="16"/>
+      <c r="AG46" s="16"/>
+      <c r="AH46" s="16"/>
+    </row>
+    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
+      <c r="W47" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="X47" s="16"/>
+      <c r="Y47" s="16"/>
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="16"/>
+      <c r="AB47" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC47" s="16"/>
+      <c r="AD47" s="16"/>
+      <c r="AE47" s="16"/>
+      <c r="AF47" s="16"/>
+      <c r="AG47" s="16"/>
+      <c r="AH47" s="16"/>
+    </row>
+    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <f>(C23/C34)*(C23/C34)</f>
+        <v>40000</v>
+      </c>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
+      <c r="T48" s="16"/>
+      <c r="U48" s="16"/>
+      <c r="V48" s="16"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="16"/>
+      <c r="Y48" s="16"/>
+      <c r="Z48" s="16"/>
+      <c r="AA48" s="16"/>
+      <c r="AB48" s="16"/>
+      <c r="AC48" s="16"/>
+      <c r="AD48" s="16"/>
+      <c r="AE48" s="16"/>
+      <c r="AF48" s="16"/>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="16"/>
+    </row>
+    <row r="49" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="R49" s="16"/>
+      <c r="S49" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="T49" s="16">
+        <f>N38+0.498-0.692</f>
+        <v>-6.9999999999998952E-3</v>
+      </c>
+      <c r="U49" s="16"/>
+      <c r="V49" s="16"/>
+      <c r="W49" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="X49" s="16"/>
+      <c r="Y49" s="16"/>
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC49" s="16"/>
+      <c r="AD49" s="16"/>
+      <c r="AE49" s="16"/>
+      <c r="AF49" s="16"/>
+      <c r="AG49" s="16"/>
+      <c r="AH49" s="16"/>
+    </row>
+    <row r="50" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
+      <c r="T50" s="16"/>
+      <c r="U50" s="16"/>
+      <c r="V50" s="16"/>
+      <c r="W50" s="16"/>
+      <c r="X50" s="16"/>
+      <c r="Y50" s="16"/>
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="16"/>
+      <c r="AB50" s="16"/>
+      <c r="AC50" s="16"/>
+      <c r="AD50" s="16"/>
+      <c r="AE50" s="16"/>
+      <c r="AF50" s="16"/>
+      <c r="AG50" s="16"/>
+      <c r="AH50" s="16"/>
+    </row>
+    <row r="51" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
+      <c r="V51" s="16"/>
+      <c r="W51" s="16"/>
+      <c r="X51" s="16"/>
+      <c r="Y51" s="16"/>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16"/>
+      <c r="AB51" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC51" s="16">
+        <f>C25+N37+N40+C10</f>
+        <v>2.2370000000000001</v>
+      </c>
+      <c r="AD51" s="16"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="16"/>
+      <c r="AH51" s="16"/>
+    </row>
+    <row r="52" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
+      <c r="T52" s="16"/>
+      <c r="U52" s="16"/>
+      <c r="V52" s="16"/>
+      <c r="W52" s="16"/>
+      <c r="X52" s="16"/>
+      <c r="Y52" s="16"/>
+      <c r="Z52" s="16"/>
+      <c r="AA52" s="16"/>
+      <c r="AB52" s="16"/>
+      <c r="AC52" s="16"/>
+      <c r="AD52" s="16"/>
+      <c r="AE52" s="16"/>
+      <c r="AF52" s="16"/>
+      <c r="AG52" s="16"/>
+      <c r="AH52" s="16"/>
+    </row>
+    <row r="53" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="16"/>
+      <c r="U53" s="16"/>
+      <c r="V53" s="16"/>
+      <c r="W53" s="16"/>
+      <c r="X53" s="16"/>
+      <c r="Y53" s="16"/>
+      <c r="Z53" s="16"/>
+      <c r="AA53" s="16"/>
+      <c r="AB53" s="16"/>
+      <c r="AC53" s="16"/>
+      <c r="AD53" s="16"/>
+      <c r="AE53" s="16"/>
+      <c r="AF53" s="16"/>
+      <c r="AG53" s="16"/>
+      <c r="AH53" s="16"/>
+    </row>
+    <row r="54" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+      <c r="T54" s="16"/>
+      <c r="U54" s="16"/>
+      <c r="V54" s="16"/>
+      <c r="W54" s="16"/>
+      <c r="X54" s="16"/>
+      <c r="Y54" s="16"/>
+      <c r="Z54" s="16"/>
+      <c r="AA54" s="16"/>
+      <c r="AB54" s="16"/>
+      <c r="AC54" s="16"/>
+      <c r="AD54" s="16"/>
+      <c r="AE54" s="16"/>
+      <c r="AF54" s="16"/>
+      <c r="AG54" s="16"/>
+      <c r="AH54" s="16"/>
+    </row>
+    <row r="55" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="3"/>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="3"/>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="3"/>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="3"/>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="3"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="3"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="3"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="3"/>
     </row>

</xml_diff>

<commit_message>
aggiunti i dubbi amletici
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C569A72-328C-4CE5-A461-031246A79835}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1270F8FF-3F05-468A-BEA1-34AE554D9F4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3265,8 +3265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AH183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
non so che sia
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1270F8FF-3F05-468A-BEA1-34AE554D9F4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5E73EB-B252-47FD-8BAD-87BA544B0482}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3265,8 +3265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AH183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4055,7 +4055,7 @@
         <v>40</v>
       </c>
       <c r="C31" s="32">
-        <f>C23/SQRT(C24)</f>
+        <f>SQRT(C23*C23/C24)</f>
         <v>0.21213203435596426</v>
       </c>
       <c r="D31" s="32"/>
@@ -6935,10 +6935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E533CDB7-452E-4AEE-B021-5A11B297142C}">
-  <dimension ref="B3:AB104"/>
+  <dimension ref="A3:AB104"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8745,7 +8745,7 @@
       </c>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C33" s="7"/>
       <c r="D33" s="9">
         <f t="shared" si="0"/>
@@ -8807,7 +8807,7 @@
       </c>
       <c r="AB33" s="7"/>
     </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C34" s="7"/>
       <c r="D34" s="9">
         <f t="shared" si="0"/>
@@ -8869,7 +8869,7 @@
       </c>
       <c r="AB34" s="7"/>
     </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -8901,7 +8901,7 @@
       <c r="AA35" s="7"/>
       <c r="AB35" s="7"/>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -8933,7 +8933,7 @@
       <c r="AA36" s="7"/>
       <c r="AB36" s="7"/>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -8965,7 +8965,7 @@
       <c r="AA37" s="7"/>
       <c r="AB37" s="7"/>
     </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -8997,7 +8997,7 @@
       <c r="AA38" s="7"/>
       <c r="AB38" s="7"/>
     </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -9025,7 +9025,7 @@
       <c r="AA39" s="7"/>
       <c r="AB39" s="7"/>
     </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C40" s="10"/>
       <c r="G40" s="5" t="s">
         <v>25</v>
@@ -9050,7 +9050,7 @@
       <c r="Z40" s="10"/>
       <c r="AB40" s="10"/>
     </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C41" s="10"/>
       <c r="D41" s="1" t="s">
         <v>12</v>
@@ -9105,7 +9105,7 @@
       </c>
       <c r="AB41" s="10"/>
     </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -9133,7 +9133,7 @@
       <c r="AA42" s="10"/>
       <c r="AB42" s="10"/>
     </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="11" t="s">
         <v>29</v>
@@ -9200,7 +9200,7 @@
       </c>
       <c r="AB43" s="10"/>
     </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="10"/>
       <c r="D44">
@@ -9263,7 +9263,11 @@
       </c>
       <c r="AB44" s="10"/>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f>(L45/0.186)*(L45/0.186)</f>
+        <v>32801.749981489193</v>
+      </c>
       <c r="B45" s="2"/>
       <c r="C45" s="10"/>
       <c r="D45">
@@ -9326,7 +9330,7 @@
       </c>
       <c r="AB45" s="10"/>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="10"/>
       <c r="D46">
@@ -9389,7 +9393,7 @@
       </c>
       <c r="AB46" s="10"/>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="10"/>
       <c r="D47">
@@ -9452,7 +9456,7 @@
       </c>
       <c r="AB47" s="10"/>
     </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="10"/>
       <c r="D48">

</xml_diff>

<commit_message>
modificati i valori di Add con Vcm
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2384D6-058E-469D-9E8D-176F4BC4C0A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F36D709-79E6-4891-8722-F7B985CDF82F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,9 +367,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Add_out(mv)</t>
-  </si>
-  <si>
     <t>Add_calc</t>
   </si>
   <si>
@@ -563,6 +560,9 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>f_p1_emp</t>
   </si>
 </sst>
 </file>
@@ -3274,8 +3274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AH183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T51" sqref="T51"/>
+    <sheetView tabSelected="1" topLeftCell="H52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB82" sqref="AB82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3320,7 +3320,7 @@
       <c r="E3" s="7"/>
       <c r="I3" s="48"/>
       <c r="J3" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K3" s="48"/>
       <c r="L3" s="48"/>
@@ -3367,14 +3367,14 @@
       <c r="E5" s="7"/>
       <c r="I5" s="48"/>
       <c r="J5" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K5" s="48"/>
       <c r="L5" s="48"/>
       <c r="M5" s="48"/>
       <c r="N5" s="48"/>
       <c r="O5" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P5" s="48"/>
       <c r="Q5" s="48"/>
@@ -3413,12 +3413,12 @@
         <v>242.3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E7" s="7"/>
       <c r="I7" s="48"/>
       <c r="J7" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K7" s="51">
         <f>T64</f>
@@ -3428,11 +3428,11 @@
       <c r="M7" s="48"/>
       <c r="N7" s="48"/>
       <c r="O7" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P7" s="48">
         <f>POWER(10,AB63/20)</f>
-        <v>53000.000000000109</v>
+        <v>26807.110220619834</v>
       </c>
       <c r="Q7" s="48"/>
       <c r="R7" s="48"/>
@@ -3448,28 +3448,28 @@
       <c r="E8" s="7"/>
       <c r="I8" s="48"/>
       <c r="J8" s="49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K8" s="51">
         <f>K84</f>
         <v>80</v>
       </c>
       <c r="L8" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M8" s="48"/>
       <c r="N8" s="48"/>
       <c r="O8" s="49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P8" s="48">
         <v>87</v>
       </c>
       <c r="Q8" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="R8" s="49" t="s">
         <v>171</v>
-      </c>
-      <c r="R8" s="49" t="s">
-        <v>172</v>
       </c>
       <c r="S8" s="48"/>
       <c r="T8" s="48"/>
@@ -3483,7 +3483,7 @@
       <c r="E9" s="7"/>
       <c r="I9" s="48"/>
       <c r="J9" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K9" s="52">
         <f>AB79</f>
@@ -3495,11 +3495,11 @@
       <c r="M9" s="48"/>
       <c r="N9" s="48"/>
       <c r="O9" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P9" s="48">
         <f>AB81</f>
-        <v>105.91551739201577</v>
+        <v>99.995000000000005</v>
       </c>
       <c r="Q9" s="49" t="s">
         <v>97</v>
@@ -3522,26 +3522,26 @@
       <c r="F10" s="1"/>
       <c r="I10" s="48"/>
       <c r="J10" s="49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K10" s="52">
         <f>E97</f>
         <v>2197335.9955648109</v>
       </c>
       <c r="L10" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M10" s="48"/>
       <c r="N10" s="48"/>
       <c r="O10" s="49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P10" s="48">
         <f>K98</f>
         <v>2187050.3597122305</v>
       </c>
       <c r="Q10" s="49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R10" s="48"/>
       <c r="S10" s="48"/>
@@ -3556,26 +3556,26 @@
       <c r="E11" s="7"/>
       <c r="I11" s="48"/>
       <c r="J11" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K11" s="51">
         <f>R95</f>
         <v>165</v>
       </c>
       <c r="L11" s="49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M11" s="48"/>
       <c r="N11" s="48"/>
       <c r="O11" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P11" s="48">
         <f>R97</f>
-        <v>167.34299999999999</v>
+        <v>167.57399999999998</v>
       </c>
       <c r="Q11" s="49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R11" s="48"/>
       <c r="S11" s="48"/>
@@ -3774,7 +3774,7 @@
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
       <c r="F23" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G23" s="35"/>
       <c r="H23" s="32"/>
@@ -4959,10 +4959,10 @@
         <v>4437692.9635714283</v>
       </c>
       <c r="R51" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T51" s="13">
         <f>0.15+0.498-0.692</f>
@@ -5005,10 +5005,10 @@
         <v>2765350.0814285716</v>
       </c>
       <c r="R52" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="T52" s="13">
         <f>C25-0.15-0.15+C10</f>
@@ -5162,7 +5162,7 @@
       <c r="E59" s="30"/>
       <c r="F59" s="13"/>
       <c r="G59" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
@@ -5202,7 +5202,7 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
       <c r="K60" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L60" s="30">
         <f>(K55*K56/(K55+K56))</f>
@@ -5241,7 +5241,7 @@
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
       <c r="K61" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L61" s="30">
         <f>(K51*K53/(K51+K53))</f>
@@ -5250,7 +5250,7 @@
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
       <c r="P61" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q61" s="24"/>
       <c r="R61" s="24"/>
@@ -5263,9 +5263,7 @@
       <c r="Y61" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="Z61" s="25" t="s">
-        <v>111</v>
-      </c>
+      <c r="Z61" s="25"/>
       <c r="AA61" s="24"/>
       <c r="AB61" s="25" t="s">
         <v>105</v>
@@ -5285,19 +5283,19 @@
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
       <c r="H62" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
       <c r="K62" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L62" s="30">
         <f>1.5*N62</f>
         <v>6635.9349147503563</v>
       </c>
       <c r="M62" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N62" s="31">
         <f>1/I55</f>
@@ -5315,13 +5313,11 @@
       <c r="Y62" s="26">
         <v>0</v>
       </c>
-      <c r="Z62" s="24">
-        <v>5</v>
-      </c>
+      <c r="Z62" s="24"/>
       <c r="AA62" s="24"/>
       <c r="AB62" s="24">
-        <f t="shared" ref="AB62:AB72" si="4">20*LOG10(Z62*1000)</f>
-        <v>73.979400086720375</v>
+        <f>69.167</f>
+        <v>69.167000000000002</v>
       </c>
       <c r="AC62" s="24"/>
       <c r="AD62" s="24"/>
@@ -5338,12 +5334,12 @@
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L63" s="30">
         <f>I50/H73</f>
@@ -5361,16 +5357,13 @@
       <c r="W63" s="24"/>
       <c r="X63" s="24"/>
       <c r="Y63" s="26">
-        <f t="shared" ref="Y63:Y72" si="5">Y62+0.2</f>
+        <f t="shared" ref="Y63:Y72" si="4">Y62+0.2</f>
         <v>0.2</v>
       </c>
-      <c r="Z63" s="24">
-        <v>53</v>
-      </c>
+      <c r="Z63" s="24"/>
       <c r="AA63" s="24"/>
       <c r="AB63" s="24">
-        <f t="shared" si="4"/>
-        <v>94.48551739201578</v>
+        <v>88.564999999999998</v>
       </c>
       <c r="AC63" s="24"/>
       <c r="AD63" s="24"/>
@@ -5390,7 +5383,7 @@
       <c r="I64" s="13"/>
       <c r="J64" s="13"/>
       <c r="K64" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L64" s="13">
         <f>5*POWER(10,-12)</f>
@@ -5420,16 +5413,13 @@
       </c>
       <c r="X64" s="24"/>
       <c r="Y64" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
-      <c r="Z64" s="24">
-        <v>73</v>
-      </c>
+      <c r="Z64" s="24"/>
       <c r="AA64" s="24"/>
       <c r="AB64" s="24">
-        <f t="shared" si="4"/>
-        <v>97.266457202409114</v>
+        <v>91.26</v>
       </c>
       <c r="AC64" s="24"/>
       <c r="AD64" s="24"/>
@@ -5462,16 +5452,13 @@
       <c r="W65" s="24"/>
       <c r="X65" s="24"/>
       <c r="Y65" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="Z65" s="24">
-        <v>86</v>
-      </c>
+      <c r="Z65" s="24"/>
       <c r="AA65" s="24"/>
       <c r="AB65" s="24">
-        <f t="shared" si="4"/>
-        <v>98.689969024871345</v>
+        <v>92.697000000000003</v>
       </c>
       <c r="AC65" s="24"/>
       <c r="AD65" s="24"/>
@@ -5516,16 +5503,13 @@
       </c>
       <c r="X66" s="24"/>
       <c r="Y66" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="Z66" s="24">
-        <v>97</v>
-      </c>
+      <c r="Z66" s="24"/>
       <c r="AA66" s="24"/>
       <c r="AB66" s="24">
-        <f t="shared" si="4"/>
-        <v>99.735434685324904</v>
+        <v>93.762</v>
       </c>
       <c r="AC66" s="24"/>
       <c r="AD66" s="24"/>
@@ -5541,7 +5525,7 @@
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H67" s="30">
         <f>1/(L61*I55*L60*L63)</f>
@@ -5549,15 +5533,20 @@
       </c>
       <c r="I67" s="13"/>
       <c r="J67" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K67" s="30">
         <f>H67/(2*PI())</f>
         <v>60.464359153074746</v>
       </c>
       <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
+      <c r="M67" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="N67" s="13">
+        <f>69.5</f>
+        <v>69.5</v>
+      </c>
       <c r="P67" s="24"/>
       <c r="Q67" s="24"/>
       <c r="R67" s="24"/>
@@ -5568,16 +5557,13 @@
       <c r="W67" s="24"/>
       <c r="X67" s="24"/>
       <c r="Y67" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Z67" s="24">
-        <v>107</v>
-      </c>
+      <c r="Z67" s="24"/>
       <c r="AA67" s="24"/>
       <c r="AB67" s="24">
-        <f t="shared" si="4"/>
-        <v>100.5876755537042</v>
+        <v>94.614000000000004</v>
       </c>
       <c r="AC67" s="24"/>
       <c r="AD67" s="24"/>
@@ -5624,16 +5610,13 @@
       </c>
       <c r="X68" s="24"/>
       <c r="Y68" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.2</v>
       </c>
-      <c r="Z68" s="24">
-        <v>115</v>
-      </c>
+      <c r="Z68" s="24"/>
       <c r="AA68" s="24"/>
       <c r="AB68" s="24">
-        <f t="shared" si="4"/>
-        <v>101.21395680707224</v>
+        <v>95.248000000000005</v>
       </c>
       <c r="AC68" s="24"/>
       <c r="AD68" s="24"/>
@@ -5649,7 +5632,7 @@
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
       <c r="G69" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H69" s="30">
         <f>I55/L64</f>
@@ -5657,10 +5640,10 @@
       </c>
       <c r="I69" s="13"/>
       <c r="J69" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K69" s="30">
-        <f t="shared" ref="K69:K71" si="6">H69/(2*PI())</f>
+        <f t="shared" ref="K69:K71" si="5">H69/(2*PI())</f>
         <v>7195140.3292756416</v>
       </c>
       <c r="L69" s="13"/>
@@ -5676,16 +5659,13 @@
       <c r="W69" s="24"/>
       <c r="X69" s="24"/>
       <c r="Y69" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4</v>
       </c>
-      <c r="Z69" s="24">
-        <v>121</v>
-      </c>
+      <c r="Z69" s="24"/>
       <c r="AA69" s="24"/>
       <c r="AB69" s="24">
-        <f t="shared" si="4"/>
-        <v>101.655707406329</v>
+        <v>95.694999999999993</v>
       </c>
       <c r="AC69" s="24"/>
       <c r="AD69" s="24"/>
@@ -5732,16 +5712,13 @@
       </c>
       <c r="X70" s="24"/>
       <c r="Y70" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.5999999999999999</v>
       </c>
-      <c r="Z70" s="24">
-        <v>125</v>
-      </c>
+      <c r="Z70" s="24"/>
       <c r="AA70" s="24"/>
       <c r="AB70" s="24">
-        <f t="shared" si="4"/>
-        <v>101.93820026016112</v>
+        <v>95.960999999999999</v>
       </c>
       <c r="AC70" s="24"/>
       <c r="AD70" s="24"/>
@@ -5757,7 +5734,7 @@
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
       <c r="G71" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H71" s="30">
         <f>I55/L63</f>
@@ -5765,10 +5742,10 @@
       </c>
       <c r="I71" s="13"/>
       <c r="J71" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K71" s="30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>3952535.2096643532</v>
       </c>
       <c r="L71" s="13"/>
@@ -5784,16 +5761,13 @@
       <c r="W71" s="24"/>
       <c r="X71" s="24"/>
       <c r="Y71" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="Z71" s="24">
-        <v>126</v>
-      </c>
+      <c r="Z71" s="24"/>
       <c r="AA71" s="24"/>
       <c r="AB71" s="24">
-        <f t="shared" si="4"/>
-        <v>102.00741090235125</v>
+        <v>96.034000000000006</v>
       </c>
       <c r="AC71" s="24"/>
       <c r="AD71" s="24"/>
@@ -5826,16 +5800,13 @@
       <c r="W72" s="24"/>
       <c r="X72" s="24"/>
       <c r="Y72" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.9999999999999998</v>
       </c>
-      <c r="Z72" s="24">
-        <v>124.5</v>
-      </c>
+      <c r="Z72" s="24"/>
       <c r="AA72" s="24"/>
       <c r="AB72" s="24">
-        <f t="shared" si="4"/>
-        <v>101.90338702863511</v>
+        <v>95.875</v>
       </c>
       <c r="AC72" s="24"/>
       <c r="AD72" s="24"/>
@@ -5847,13 +5818,13 @@
     <row r="73" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B73" s="13"/>
       <c r="C73" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H73" s="30">
         <f>2*PI()*K73</f>
@@ -5861,7 +5832,7 @@
       </c>
       <c r="I73" s="13"/>
       <c r="J73" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K73" s="30">
         <f>H86</f>
@@ -5869,7 +5840,7 @@
       </c>
       <c r="L73" s="13"/>
       <c r="M73" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N73" s="13">
         <f>1.82*POWER(10,6)*2*PI()</f>
@@ -5880,7 +5851,7 @@
       <c r="R73" s="24"/>
       <c r="S73" s="24"/>
       <c r="T73" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U73" s="24"/>
       <c r="V73" s="24"/>
@@ -5915,7 +5886,7 @@
       <c r="Q74" s="24"/>
       <c r="R74" s="24"/>
       <c r="S74" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T74" s="28">
         <f>I55*(K55*K56/(K55+K56))*I50*(K51*K53/(K51+K53))</f>
@@ -5948,7 +5919,7 @@
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
       <c r="G75" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H75" s="30">
         <f>1/(L63*(1/I55-L62))</f>
@@ -6036,7 +6007,7 @@
       <c r="U77" s="24"/>
       <c r="V77" s="24"/>
       <c r="W77" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="X77" s="28">
         <f>K54</f>
@@ -6072,7 +6043,7 @@
       <c r="R78" s="24"/>
       <c r="S78" s="24"/>
       <c r="T78" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U78" s="24"/>
       <c r="V78" s="24"/>
@@ -6096,7 +6067,7 @@
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H79" s="30">
         <f>((PI()/2)-ATAN(H73/H69)-ATAN(H73/H71))*57</f>
@@ -6112,7 +6083,7 @@
       <c r="Q79" s="24"/>
       <c r="R79" s="24"/>
       <c r="S79" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T79" s="28">
         <f>1/(2*X77*I52)</f>
@@ -6129,7 +6100,7 @@
       <c r="X79" s="24"/>
       <c r="Y79" s="24"/>
       <c r="Z79" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AA79" s="24"/>
       <c r="AB79" s="28">
@@ -6197,7 +6168,7 @@
       <c r="Q81" s="24"/>
       <c r="R81" s="24"/>
       <c r="S81" s="25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T81" s="24"/>
       <c r="U81" s="24"/>
@@ -6210,18 +6181,18 @@
       <c r="X81" s="24"/>
       <c r="Y81" s="24"/>
       <c r="Z81" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AA81" s="24"/>
       <c r="AB81" s="26">
         <f>AB63-V81</f>
-        <v>105.91551739201577</v>
+        <v>99.995000000000005</v>
       </c>
       <c r="AC81" s="24" t="s">
         <v>97</v>
       </c>
       <c r="AD81" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AE81" s="24"/>
       <c r="AF81" s="24"/>
@@ -6303,7 +6274,7 @@
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
@@ -6337,7 +6308,7 @@
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H86" s="30">
         <f>K69*TAN((90-K84)/57)</f>
@@ -6400,7 +6371,7 @@
       <c r="C91" s="2"/>
       <c r="P91" s="42"/>
       <c r="Q91" s="43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R91" s="42"/>
       <c r="S91" s="42"/>
@@ -6430,18 +6401,19 @@
       <c r="T92" s="42"/>
       <c r="U92" s="42"/>
       <c r="V92" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W92" s="42"/>
       <c r="X92" s="42"/>
       <c r="Y92" s="42">
-        <v>50.71</v>
+        <f>L36+L37+L42</f>
+        <v>50.78</v>
       </c>
     </row>
     <row r="93" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C93" s="37"/>
       <c r="D93" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -6458,7 +6430,7 @@
       <c r="T93" s="42"/>
       <c r="U93" s="42"/>
       <c r="V93" s="46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W93" s="42"/>
       <c r="X93" s="42"/>
@@ -6480,7 +6452,7 @@
       <c r="L94" s="7"/>
       <c r="P94" s="42"/>
       <c r="Q94" s="46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R94" s="42"/>
       <c r="S94" s="42"/>
@@ -6494,17 +6466,17 @@
     <row r="95" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
       <c r="D95" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E95" s="40"/>
       <c r="F95" s="40"/>
       <c r="G95" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="38"/>
       <c r="J95" s="40" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K95" s="7"/>
       <c r="L95" s="7"/>
@@ -6517,19 +6489,19 @@
         <v>165</v>
       </c>
       <c r="S95" s="43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T95" s="42"/>
       <c r="U95" s="42"/>
       <c r="V95" s="46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="W95" s="42"/>
       <c r="X95" s="42">
         <v>3.3</v>
       </c>
       <c r="Y95" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="2:34" x14ac:dyDescent="0.25">
@@ -6557,41 +6529,41 @@
     </row>
     <row r="97" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C97" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E97" s="37">
         <f>C37*POWER(10,-6)/L63</f>
         <v>2197335.9955648109</v>
       </c>
       <c r="F97" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H97" s="37">
         <f>L37*POWER(10,-6)/L63</f>
         <v>2235789.3754871953</v>
       </c>
       <c r="I97" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
       <c r="L97" s="7"/>
       <c r="P97" s="42"/>
       <c r="Q97" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R97" s="42">
         <f>Y92*X95</f>
-        <v>167.34299999999999</v>
+        <v>167.57399999999998</v>
       </c>
       <c r="S97" s="43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T97" s="42"/>
       <c r="U97" s="42"/>
@@ -6610,25 +6582,25 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K98" s="7">
         <f>(3.04)/(1.39*POWER(10,-6))</f>
         <v>2187050.3597122305</v>
       </c>
       <c r="L98" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P98" s="42"/>
       <c r="Q98" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R98" s="42">
         <f>Y93*X95</f>
         <v>167.81819999999999</v>
       </c>
       <c r="S98" s="43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T98" s="42"/>
       <c r="U98" s="42"/>
@@ -6662,27 +6634,27 @@
     <row r="100" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B100" s="3"/>
       <c r="C100" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D100" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E100" s="37">
         <f>H73*C34</f>
         <v>1202052.6563737299</v>
       </c>
       <c r="F100" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G100" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H100" s="37">
         <f>N73*C34</f>
         <v>1715309.5888600268</v>
       </c>
       <c r="I100" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>

</xml_diff>

<commit_message>
aggiunta Ft contando lo zero
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F36D709-79E6-4891-8722-F7B985CDF82F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46164EB3-FCB2-46E0-8CEC-9DA4B85C5510}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="178">
   <si>
     <t>Vdd</t>
   </si>
@@ -547,9 +547,6 @@
     <t>°</t>
   </si>
   <si>
-    <t>da ricontrollare</t>
-  </si>
-  <si>
     <t>Empirico con Vcm = 0.2V</t>
   </si>
   <si>
@@ -563,6 +560,12 @@
   </si>
   <si>
     <t>f_p1_emp</t>
+  </si>
+  <si>
+    <t>PM_emp</t>
+  </si>
+  <si>
+    <t>fz_res</t>
   </si>
 </sst>
 </file>
@@ -679,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -745,6 +748,12 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -3274,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AH183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB82" sqref="AB82"/>
+    <sheetView tabSelected="1" topLeftCell="H19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE25" sqref="AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3374,7 +3383,7 @@
       <c r="M5" s="48"/>
       <c r="N5" s="48"/>
       <c r="O5" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P5" s="48"/>
       <c r="Q5" s="48"/>
@@ -3463,14 +3472,13 @@
         <v>124</v>
       </c>
       <c r="P8" s="48">
-        <v>87</v>
+        <f>M84</f>
+        <v>86.65</v>
       </c>
       <c r="Q8" s="49" t="s">
         <v>170</v>
       </c>
-      <c r="R8" s="49" t="s">
-        <v>171</v>
-      </c>
+      <c r="R8" s="49"/>
       <c r="S8" s="48"/>
       <c r="T8" s="48"/>
       <c r="U8" s="48"/>
@@ -3487,7 +3495,7 @@
       </c>
       <c r="K9" s="52">
         <f>AB79</f>
-        <v>137.88271077549695</v>
+        <v>136.64186441850461</v>
       </c>
       <c r="L9" s="49" t="s">
         <v>97</v>
@@ -3499,7 +3507,7 @@
       </c>
       <c r="P9" s="48">
         <f>AB81</f>
-        <v>99.995000000000005</v>
+        <v>98.05</v>
       </c>
       <c r="Q9" s="49" t="s">
         <v>97</v>
@@ -4921,7 +4929,7 @@
       </c>
       <c r="J50" s="10"/>
       <c r="K50" s="23">
-        <f>E54/J40</f>
+        <f>E54/J41</f>
         <v>3169780.6882653064</v>
       </c>
       <c r="R50" s="13"/>
@@ -4955,14 +4963,14 @@
       </c>
       <c r="J51" s="10"/>
       <c r="K51" s="23">
-        <f>E54/H40</f>
-        <v>4437692.9635714283</v>
+        <f>E54/J40</f>
+        <v>3169780.6882653064</v>
       </c>
       <c r="R51" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T51" s="13">
         <f>0.15+0.498-0.692</f>
@@ -5005,10 +5013,10 @@
         <v>2765350.0814285716</v>
       </c>
       <c r="R52" s="16" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T52" s="13">
         <f>C25-0.15-0.15+C10</f>
@@ -5245,7 +5253,7 @@
       </c>
       <c r="L61" s="30">
         <f>(K51*K53/(K51+K53))</f>
-        <v>1703693.0810354818</v>
+        <v>1476893.033118003</v>
       </c>
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
@@ -5367,7 +5375,10 @@
       </c>
       <c r="AC63" s="24"/>
       <c r="AD63" s="24"/>
-      <c r="AE63" s="24"/>
+      <c r="AE63" s="24">
+        <f>20*LOG10(50*1000)</f>
+        <v>93.979400086720375</v>
+      </c>
       <c r="AF63" s="24"/>
       <c r="AG63" s="24"/>
       <c r="AH63" s="24"/>
@@ -5529,7 +5540,7 @@
       </c>
       <c r="H67" s="30">
         <f>1/(L61*I55*L60*L63)</f>
-        <v>379.90877303862879</v>
+        <v>438.24971310490042</v>
       </c>
       <c r="I67" s="13"/>
       <c r="J67" s="14" t="s">
@@ -5537,11 +5548,11 @@
       </c>
       <c r="K67" s="30">
         <f>H67/(2*PI())</f>
-        <v>60.464359153074746</v>
+        <v>69.74960814924988</v>
       </c>
       <c r="L67" s="13"/>
       <c r="M67" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N67" s="13">
         <f>69.5</f>
@@ -5643,7 +5654,7 @@
         <v>128</v>
       </c>
       <c r="K69" s="30">
-        <f t="shared" ref="K69:K71" si="5">H69/(2*PI())</f>
+        <f t="shared" ref="K69" si="5">H69/(2*PI())</f>
         <v>7195140.3292756416</v>
       </c>
       <c r="L69" s="13"/>
@@ -5745,7 +5756,7 @@
         <v>129</v>
       </c>
       <c r="K71" s="30">
-        <f t="shared" si="5"/>
+        <f>H71/(2*PI())</f>
         <v>3952535.2096643532</v>
       </c>
       <c r="L71" s="13"/>
@@ -5890,12 +5901,12 @@
       </c>
       <c r="T74" s="28">
         <f>I55*(K55*K56/(K55+K56))*I50*(K51*K53/(K51+K53))</f>
-        <v>21093.707080594424</v>
+        <v>18285.658007736543</v>
       </c>
       <c r="U74" s="24"/>
       <c r="V74" s="28">
         <f>20*LOG10(T74)</f>
-        <v>86.483058217044331</v>
+        <v>85.242211860051981</v>
       </c>
       <c r="W74" s="25" t="s">
         <v>97</v>
@@ -5926,8 +5937,13 @@
         <v>-49669022.310946092</v>
       </c>
       <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
-      <c r="K75" s="13"/>
+      <c r="J75" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="K75" s="30">
+        <f>ABS(H75)/(2*PI())</f>
+        <v>7905070.4193287054</v>
+      </c>
       <c r="L75" s="13"/>
       <c r="M75" s="13"/>
       <c r="N75" s="13"/>
@@ -6105,7 +6121,7 @@
       <c r="AA79" s="24"/>
       <c r="AB79" s="28">
         <f>V74-V79</f>
-        <v>137.88271077549695</v>
+        <v>136.64186441850461</v>
       </c>
       <c r="AC79" s="24" t="s">
         <v>97</v>
@@ -6173,7 +6189,7 @@
       <c r="T81" s="24"/>
       <c r="U81" s="24"/>
       <c r="V81" s="24">
-        <v>-11.43</v>
+        <v>-9.4849999999999994</v>
       </c>
       <c r="W81" s="24" t="s">
         <v>97</v>
@@ -6186,7 +6202,7 @@
       <c r="AA81" s="24"/>
       <c r="AB81" s="26">
         <f>AB63-V81</f>
-        <v>99.995000000000005</v>
+        <v>98.05</v>
       </c>
       <c r="AC81" s="24" t="s">
         <v>97</v>
@@ -6279,11 +6295,16 @@
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
       <c r="J84" s="13"/>
-      <c r="K84" s="15">
+      <c r="K84" s="54">
         <v>80</v>
       </c>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
+      <c r="L84" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="M84" s="29">
+        <f>180-93.35</f>
+        <v>86.65</v>
+      </c>
       <c r="N84" s="13"/>
     </row>
     <row r="85" spans="2:34" x14ac:dyDescent="0.25">
@@ -6335,6 +6356,9 @@
       <c r="L87" s="13"/>
       <c r="M87" s="13"/>
       <c r="N87" s="13"/>
+      <c r="W87">
+        <v>-11.43</v>
+      </c>
     </row>
     <row r="88" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B88" s="13"/>

</xml_diff>

<commit_message>
modifica inutile al foglio di lavoro
</commit_message>
<xml_diff>
--- a/MicroB/CalcoliExcel.xlsx
+++ b/MicroB/CalcoliExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github-Repo\MicroElectronics\MicroB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46164EB3-FCB2-46E0-8CEC-9DA4B85C5510}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC776CF-8B9F-429A-BAFD-81BD78DA2C86}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="178">
   <si>
     <t>Vdd</t>
   </si>
@@ -376,9 +376,6 @@
     <t>Acm_calc</t>
   </si>
   <si>
-    <t xml:space="preserve"> -1/(2* Rss * GM3)</t>
-  </si>
-  <si>
     <t>Acm(0)_emp</t>
   </si>
   <si>
@@ -566,6 +563,9 @@
   </si>
   <si>
     <t>fz_res</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1/(2* Rss * GM3)</t>
   </si>
 </sst>
 </file>
@@ -3283,8 +3283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AH183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE25" sqref="AE25"/>
+    <sheetView topLeftCell="F13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X78" sqref="X78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,7 +3329,7 @@
       <c r="E3" s="7"/>
       <c r="I3" s="48"/>
       <c r="J3" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K3" s="48"/>
       <c r="L3" s="48"/>
@@ -3376,14 +3376,14 @@
       <c r="E5" s="7"/>
       <c r="I5" s="48"/>
       <c r="J5" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K5" s="48"/>
       <c r="L5" s="48"/>
       <c r="M5" s="48"/>
       <c r="N5" s="48"/>
       <c r="O5" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P5" s="48"/>
       <c r="Q5" s="48"/>
@@ -3422,12 +3422,12 @@
         <v>242.3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" s="7"/>
       <c r="I7" s="48"/>
       <c r="J7" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K7" s="51">
         <f>T64</f>
@@ -3437,7 +3437,7 @@
       <c r="M7" s="48"/>
       <c r="N7" s="48"/>
       <c r="O7" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P7" s="48">
         <f>POWER(10,AB63/20)</f>
@@ -3457,26 +3457,26 @@
       <c r="E8" s="7"/>
       <c r="I8" s="48"/>
       <c r="J8" s="49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K8" s="51">
         <f>K84</f>
         <v>80</v>
       </c>
       <c r="L8" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M8" s="48"/>
       <c r="N8" s="48"/>
       <c r="O8" s="49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="P8" s="48">
         <f>M84</f>
         <v>86.65</v>
       </c>
       <c r="Q8" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R8" s="49"/>
       <c r="S8" s="48"/>
@@ -3491,11 +3491,11 @@
       <c r="E9" s="7"/>
       <c r="I9" s="48"/>
       <c r="J9" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K9" s="52">
         <f>AB79</f>
-        <v>136.64186441850461</v>
+        <v>116.45138369405188</v>
       </c>
       <c r="L9" s="49" t="s">
         <v>97</v>
@@ -3503,7 +3503,7 @@
       <c r="M9" s="48"/>
       <c r="N9" s="48"/>
       <c r="O9" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P9" s="48">
         <f>AB81</f>
@@ -3530,26 +3530,26 @@
       <c r="F10" s="1"/>
       <c r="I10" s="48"/>
       <c r="J10" s="49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K10" s="52">
         <f>E97</f>
         <v>2197335.9955648109</v>
       </c>
       <c r="L10" s="49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M10" s="48"/>
       <c r="N10" s="48"/>
       <c r="O10" s="49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P10" s="48">
         <f>K98</f>
         <v>2187050.3597122305</v>
       </c>
       <c r="Q10" s="49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="R10" s="48"/>
       <c r="S10" s="48"/>
@@ -3564,26 +3564,26 @@
       <c r="E11" s="7"/>
       <c r="I11" s="48"/>
       <c r="J11" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K11" s="51">
         <f>R95</f>
         <v>165</v>
       </c>
       <c r="L11" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M11" s="48"/>
       <c r="N11" s="48"/>
       <c r="O11" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P11" s="48">
         <f>R97</f>
         <v>167.57399999999998</v>
       </c>
       <c r="Q11" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R11" s="48"/>
       <c r="S11" s="48"/>
@@ -3782,7 +3782,7 @@
       <c r="D23" s="35"/>
       <c r="E23" s="35"/>
       <c r="F23" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G23" s="35"/>
       <c r="H23" s="32"/>
@@ -4967,10 +4967,10 @@
         <v>3169780.6882653064</v>
       </c>
       <c r="R51" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S51" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T51" s="13">
         <f>0.15+0.498-0.692</f>
@@ -5013,10 +5013,10 @@
         <v>2765350.0814285716</v>
       </c>
       <c r="R52" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S52" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T52" s="13">
         <f>C25-0.15-0.15+C10</f>
@@ -5170,7 +5170,7 @@
       <c r="E59" s="30"/>
       <c r="F59" s="13"/>
       <c r="G59" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
@@ -5210,7 +5210,7 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
       <c r="K60" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L60" s="30">
         <f>(K55*K56/(K55+K56))</f>
@@ -5249,7 +5249,7 @@
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
       <c r="K61" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L61" s="30">
         <f>(K51*K53/(K51+K53))</f>
@@ -5258,7 +5258,7 @@
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
       <c r="P61" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q61" s="24"/>
       <c r="R61" s="24"/>
@@ -5291,19 +5291,19 @@
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
       <c r="H62" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
       <c r="K62" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L62" s="30">
         <f>1.5*N62</f>
         <v>6635.9349147503563</v>
       </c>
       <c r="M62" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N62" s="31">
         <f>1/I55</f>
@@ -5342,12 +5342,12 @@
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
       <c r="K63" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L63" s="30">
         <f>I50/H73</f>
@@ -5394,7 +5394,7 @@
       <c r="I64" s="13"/>
       <c r="J64" s="13"/>
       <c r="K64" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L64" s="13">
         <f>5*POWER(10,-12)</f>
@@ -5536,7 +5536,7 @@
       <c r="E67" s="13"/>
       <c r="F67" s="13"/>
       <c r="G67" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H67" s="30">
         <f>1/(L61*I55*L60*L63)</f>
@@ -5544,7 +5544,7 @@
       </c>
       <c r="I67" s="13"/>
       <c r="J67" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K67" s="30">
         <f>H67/(2*PI())</f>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="L67" s="13"/>
       <c r="M67" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="N67" s="13">
         <f>69.5</f>
@@ -5643,7 +5643,7 @@
       <c r="E69" s="13"/>
       <c r="F69" s="13"/>
       <c r="G69" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H69" s="30">
         <f>I55/L64</f>
@@ -5651,7 +5651,7 @@
       </c>
       <c r="I69" s="13"/>
       <c r="J69" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K69" s="30">
         <f t="shared" ref="K69" si="5">H69/(2*PI())</f>
@@ -5745,7 +5745,7 @@
       <c r="E71" s="13"/>
       <c r="F71" s="13"/>
       <c r="G71" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H71" s="30">
         <f>I55/L63</f>
@@ -5753,7 +5753,7 @@
       </c>
       <c r="I71" s="13"/>
       <c r="J71" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K71" s="30">
         <f>H71/(2*PI())</f>
@@ -5829,13 +5829,13 @@
     <row r="73" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B73" s="13"/>
       <c r="C73" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H73" s="30">
         <f>2*PI()*K73</f>
@@ -5843,7 +5843,7 @@
       </c>
       <c r="I73" s="13"/>
       <c r="J73" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K73" s="30">
         <f>H86</f>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="L73" s="13"/>
       <c r="M73" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N73" s="13">
         <f>1.82*POWER(10,6)*2*PI()</f>
@@ -5930,7 +5930,7 @@
       <c r="E75" s="13"/>
       <c r="F75" s="13"/>
       <c r="G75" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H75" s="30">
         <f>1/(L63*(1/I55-L62))</f>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="I75" s="13"/>
       <c r="J75" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K75" s="30">
         <f>ABS(H75)/(2*PI())</f>
@@ -6023,16 +6023,19 @@
       <c r="U77" s="24"/>
       <c r="V77" s="24"/>
       <c r="W77" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X77" s="28">
-        <f>K54</f>
-        <v>1643589.9865079366</v>
+        <f>2.3/(L37*POWER(10,-6))</f>
+        <v>113022.11302211302</v>
       </c>
       <c r="Y77" s="24"/>
       <c r="Z77" s="24"/>
       <c r="AA77" s="24"/>
-      <c r="AB77" s="24"/>
+      <c r="AB77" s="28">
+        <f>V66-V79</f>
+        <v>116.45138369405188</v>
+      </c>
       <c r="AC77" s="24"/>
       <c r="AD77" s="24"/>
       <c r="AE77" s="24"/>
@@ -6059,7 +6062,7 @@
       <c r="R78" s="24"/>
       <c r="S78" s="24"/>
       <c r="T78" s="24" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="U78" s="24"/>
       <c r="V78" s="24"/>
@@ -6083,7 +6086,7 @@
       <c r="E79" s="13"/>
       <c r="F79" s="13"/>
       <c r="G79" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H79" s="30">
         <f>((PI()/2)-ATAN(H73/H69)-ATAN(H73/H71))*57</f>
@@ -6103,12 +6106,12 @@
       </c>
       <c r="T79" s="28">
         <f>1/(2*X77*I52)</f>
-        <v>2.6916424693198314E-3</v>
+        <v>3.9142398700049208E-2</v>
       </c>
       <c r="U79" s="24"/>
       <c r="V79" s="28">
         <f>20*LOG10(T79)</f>
-        <v>-51.399652558452615</v>
+        <v>-28.147051273982036</v>
       </c>
       <c r="W79" s="24" t="s">
         <v>97</v>
@@ -6116,12 +6119,12 @@
       <c r="X79" s="24"/>
       <c r="Y79" s="24"/>
       <c r="Z79" s="25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AA79" s="24"/>
       <c r="AB79" s="28">
-        <f>V74-V79</f>
-        <v>136.64186441850461</v>
+        <f>V66-V79</f>
+        <v>116.45138369405188</v>
       </c>
       <c r="AC79" s="24" t="s">
         <v>97</v>
@@ -6184,7 +6187,7 @@
       <c r="Q81" s="24"/>
       <c r="R81" s="24"/>
       <c r="S81" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T81" s="24"/>
       <c r="U81" s="24"/>
@@ -6197,7 +6200,7 @@
       <c r="X81" s="24"/>
       <c r="Y81" s="24"/>
       <c r="Z81" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AA81" s="24"/>
       <c r="AB81" s="26">
@@ -6208,7 +6211,7 @@
         <v>97</v>
       </c>
       <c r="AD81" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AE81" s="24"/>
       <c r="AF81" s="24"/>
@@ -6290,7 +6293,7 @@
       <c r="E84" s="13"/>
       <c r="F84" s="13"/>
       <c r="G84" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H84" s="13"/>
       <c r="I84" s="13"/>
@@ -6299,7 +6302,7 @@
         <v>80</v>
       </c>
       <c r="L84" s="53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M84" s="29">
         <f>180-93.35</f>
@@ -6329,7 +6332,7 @@
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H86" s="30">
         <f>K69*TAN((90-K84)/57)</f>
@@ -6395,7 +6398,7 @@
       <c r="C91" s="2"/>
       <c r="P91" s="42"/>
       <c r="Q91" s="43" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R91" s="42"/>
       <c r="S91" s="42"/>
@@ -6425,7 +6428,7 @@
       <c r="T92" s="42"/>
       <c r="U92" s="42"/>
       <c r="V92" s="46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="W92" s="42"/>
       <c r="X92" s="42"/>
@@ -6437,7 +6440,7 @@
     <row r="93" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C93" s="37"/>
       <c r="D93" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -6454,7 +6457,7 @@
       <c r="T93" s="42"/>
       <c r="U93" s="42"/>
       <c r="V93" s="46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W93" s="42"/>
       <c r="X93" s="42"/>
@@ -6476,7 +6479,7 @@
       <c r="L94" s="7"/>
       <c r="P94" s="42"/>
       <c r="Q94" s="46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R94" s="42"/>
       <c r="S94" s="42"/>
@@ -6490,17 +6493,17 @@
     <row r="95" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C95" s="7"/>
       <c r="D95" s="40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E95" s="40"/>
       <c r="F95" s="40"/>
       <c r="G95" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H95" s="7"/>
       <c r="I95" s="38"/>
       <c r="J95" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K95" s="7"/>
       <c r="L95" s="7"/>
@@ -6513,19 +6516,19 @@
         <v>165</v>
       </c>
       <c r="S95" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="T95" s="42"/>
       <c r="U95" s="42"/>
       <c r="V95" s="46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="W95" s="42"/>
       <c r="X95" s="42">
         <v>3.3</v>
       </c>
       <c r="Y95" s="43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="2:34" x14ac:dyDescent="0.25">
@@ -6553,41 +6556,41 @@
     </row>
     <row r="97" spans="2:25" x14ac:dyDescent="0.25">
       <c r="C97" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E97" s="37">
         <f>C37*POWER(10,-6)/L63</f>
         <v>2197335.9955648109</v>
       </c>
       <c r="F97" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H97" s="37">
         <f>L37*POWER(10,-6)/L63</f>
         <v>2235789.3754871953</v>
       </c>
       <c r="I97" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
       <c r="L97" s="7"/>
       <c r="P97" s="42"/>
       <c r="Q97" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R97" s="42">
         <f>Y92*X95</f>
         <v>167.57399999999998</v>
       </c>
       <c r="S97" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="T97" s="42"/>
       <c r="U97" s="42"/>
@@ -6606,25 +6609,25 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K98" s="7">
         <f>(3.04)/(1.39*POWER(10,-6))</f>
         <v>2187050.3597122305</v>
       </c>
       <c r="L98" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P98" s="42"/>
       <c r="Q98" s="43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R98" s="42">
         <f>Y93*X95</f>
         <v>167.81819999999999</v>
       </c>
       <c r="S98" s="43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="T98" s="42"/>
       <c r="U98" s="42"/>
@@ -6658,27 +6661,27 @@
     <row r="100" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B100" s="3"/>
       <c r="C100" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D100" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E100" s="37">
         <f>H73*C34</f>
         <v>1202052.6563737299</v>
       </c>
       <c r="F100" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G100" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H100" s="37">
         <f>N73*C34</f>
         <v>1715309.5888600268</v>
       </c>
       <c r="I100" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
@@ -6954,10 +6957,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E533CDB7-452E-4AEE-B021-5A11B297142C}">
-  <dimension ref="A3:AB104"/>
+  <dimension ref="A3:AM104"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6975,6 +6978,8 @@
     <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="14" customWidth="1"/>
     <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.140625" customWidth="1"/>
+    <col min="39" max="39" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:28" x14ac:dyDescent="0.25">
@@ -9538,7 +9543,7 @@
       </c>
       <c r="AB48" s="10"/>
     </row>
-    <row r="49" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="10"/>
       <c r="D49">
@@ -9601,7 +9606,7 @@
       </c>
       <c r="AB49" s="10"/>
     </row>
-    <row r="50" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="10"/>
       <c r="D50">
@@ -9664,7 +9669,7 @@
       </c>
       <c r="AB50" s="10"/>
     </row>
-    <row r="51" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="10"/>
       <c r="D51">
@@ -9727,7 +9732,7 @@
       </c>
       <c r="AB51" s="10"/>
     </row>
-    <row r="52" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="10"/>
       <c r="D52">
@@ -9790,7 +9795,7 @@
       </c>
       <c r="AB52" s="10"/>
     </row>
-    <row r="53" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="10"/>
       <c r="D53">
@@ -9853,7 +9858,7 @@
       </c>
       <c r="AB53" s="10"/>
     </row>
-    <row r="54" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="10"/>
       <c r="D54">
@@ -9916,7 +9921,7 @@
       </c>
       <c r="AB54" s="10"/>
     </row>
-    <row r="55" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="10"/>
       <c r="D55">
@@ -9979,7 +9984,7 @@
       </c>
       <c r="AB55" s="10"/>
     </row>
-    <row r="56" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="10"/>
       <c r="D56">
@@ -10042,7 +10047,7 @@
       </c>
       <c r="AB56" s="10"/>
     </row>
-    <row r="57" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="10"/>
       <c r="D57">
@@ -10105,7 +10110,7 @@
       </c>
       <c r="AB57" s="10"/>
     </row>
-    <row r="58" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="10"/>
       <c r="D58">
@@ -10168,7 +10173,7 @@
       </c>
       <c r="AB58" s="10"/>
     </row>
-    <row r="59" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="10"/>
       <c r="D59">
@@ -10230,8 +10235,18 @@
         <v>5.193362709694301E-5</v>
       </c>
       <c r="AB59" s="10"/>
-    </row>
-    <row r="60" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AF59" s="1"/>
+      <c r="AG59" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH59" s="1"/>
+      <c r="AI59" s="1"/>
+      <c r="AJ59" s="1"/>
+      <c r="AK59" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="10"/>
       <c r="D60">
@@ -10294,7 +10309,7 @@
       </c>
       <c r="AB60" s="10"/>
     </row>
-    <row r="61" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="10"/>
       <c r="D61">
@@ -10356,8 +10371,26 @@
         <v>5.7175505156340349E-5</v>
       </c>
       <c r="AB61" s="10"/>
-    </row>
-    <row r="62" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH61" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL61" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM61" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="10"/>
       <c r="D62">
@@ -10420,7 +10453,7 @@
       </c>
       <c r="AB62" s="10"/>
     </row>
-    <row r="63" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="10"/>
       <c r="D63">
@@ -10482,8 +10515,26 @@
         <v>6.2088159562748979E-5</v>
       </c>
       <c r="AB63" s="10"/>
-    </row>
-    <row r="64" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG63">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AH63">
+        <v>33.686931328923386</v>
+      </c>
+      <c r="AI63">
+        <v>62127701.48724293</v>
+      </c>
+      <c r="AK63" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="AL63">
+        <v>30.698603243027605</v>
+      </c>
+      <c r="AM63">
+        <v>46371199.127336897</v>
+      </c>
+    </row>
+    <row r="64" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="10"/>
       <c r="D64">
@@ -10545,8 +10596,26 @@
         <v>6.4425760561130223E-5</v>
       </c>
       <c r="AB64" s="10"/>
-    </row>
-    <row r="65" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG64">
+        <v>1.2</v>
+      </c>
+      <c r="AH64">
+        <v>39.607537574373495</v>
+      </c>
+      <c r="AI64">
+        <v>9378772.7962928712</v>
+      </c>
+      <c r="AK64" s="9">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AL64">
+        <v>67.132260400883141</v>
+      </c>
+      <c r="AM64">
+        <v>7663594.617599722</v>
+      </c>
+    </row>
+    <row r="65" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="10"/>
       <c r="D65">
@@ -10608,8 +10677,26 @@
         <v>6.6686754797811389E-5</v>
       </c>
       <c r="AB65" s="10"/>
-    </row>
-    <row r="66" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG65">
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="AH65">
+        <v>40.925107655850319</v>
+      </c>
+      <c r="AI65">
+        <v>3697543.1109455386</v>
+      </c>
+      <c r="AK65" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="AL65">
+        <v>93.880034496879716</v>
+      </c>
+      <c r="AM65">
+        <v>3678565.5347506325</v>
+      </c>
+    </row>
+    <row r="66" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="10"/>
       <c r="D66">
@@ -10671,8 +10758,26 @@
         <v>6.8873079877792155E-5</v>
       </c>
       <c r="AB66" s="10"/>
-    </row>
-    <row r="67" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG66">
+        <v>1.8000000000000005</v>
+      </c>
+      <c r="AH66">
+        <v>41.131882971376498</v>
+      </c>
+      <c r="AI66">
+        <v>1990782.9949059791</v>
+      </c>
+      <c r="AK66" s="9">
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="AL66">
+        <v>114.66366549828025</v>
+      </c>
+      <c r="AM66">
+        <v>2306356.1320470562</v>
+      </c>
+    </row>
+    <row r="67" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="10"/>
       <c r="D67">
@@ -10734,8 +10839,26 @@
         <v>7.0986653702485183E-5</v>
       </c>
       <c r="AB67" s="10"/>
-    </row>
-    <row r="68" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG67">
+        <v>2.1000000000000005</v>
+      </c>
+      <c r="AH67">
+        <v>40.84268062645635</v>
+      </c>
+      <c r="AI67">
+        <v>1251733.5411369323</v>
+      </c>
+      <c r="AK67" s="9">
+        <v>1.8000000000000005</v>
+      </c>
+      <c r="AL67">
+        <v>130.81037277990555</v>
+      </c>
+      <c r="AM67">
+        <v>1630610.9025091648</v>
+      </c>
+    </row>
+    <row r="68" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="10"/>
       <c r="D68">
@@ -10797,8 +10920,26 @@
         <v>7.3029401606658731E-5</v>
       </c>
       <c r="AB68" s="10"/>
-    </row>
-    <row r="69" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG68">
+        <v>2.4000000000000008</v>
+      </c>
+      <c r="AH68">
+        <v>40.248862499406975</v>
+      </c>
+      <c r="AI68">
+        <v>863236.43981653475</v>
+      </c>
+      <c r="AK68" s="9">
+        <v>2.1000000000000005</v>
+      </c>
+      <c r="AL68">
+        <v>142.89707801635609</v>
+      </c>
+      <c r="AM68">
+        <v>1232102.7142081733</v>
+      </c>
+    </row>
+    <row r="69" spans="2:39" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="10"/>
       <c r="D69">
@@ -10860,8 +11001,26 @@
         <v>7.5003232614442899E-5</v>
       </c>
       <c r="AB69" s="10"/>
-    </row>
-    <row r="70" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG69">
+        <v>2.7000000000000011</v>
+      </c>
+      <c r="AH69">
+        <v>39.427965619924429</v>
+      </c>
+      <c r="AI69">
+        <v>632501.95154954342</v>
+      </c>
+      <c r="AK69" s="9">
+        <v>2.4000000000000008</v>
+      </c>
+      <c r="AL69">
+        <v>151.34088842449563</v>
+      </c>
+      <c r="AM69">
+        <v>969873.28605536313</v>
+      </c>
+    </row>
+    <row r="70" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="10"/>
@@ -10892,8 +11051,26 @@
       <c r="Z70" s="10"/>
       <c r="AA70" s="10"/>
       <c r="AB70" s="10"/>
-    </row>
-    <row r="71" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG70">
+        <v>3.0000000000000013</v>
+      </c>
+      <c r="AH70">
+        <v>38.416416120705669</v>
+      </c>
+      <c r="AI70">
+        <v>483349.78957223747</v>
+      </c>
+      <c r="AK70" s="9">
+        <v>2.7000000000000011</v>
+      </c>
+      <c r="AL70">
+        <v>156.74473379542886</v>
+      </c>
+      <c r="AM70">
+        <v>785291.88476882654</v>
+      </c>
+    </row>
+    <row r="71" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
       <c r="E71" s="10"/>
@@ -10924,8 +11101,26 @@
       <c r="Z71" s="10"/>
       <c r="AA71" s="10"/>
       <c r="AB71" s="10"/>
-    </row>
-    <row r="72" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG71">
+        <v>3.3000000000000016</v>
+      </c>
+      <c r="AH71">
+        <v>37.23009576946216</v>
+      </c>
+      <c r="AI71">
+        <v>380659.41886181786</v>
+      </c>
+      <c r="AK71" s="9">
+        <v>3.0000000000000013</v>
+      </c>
+      <c r="AL71">
+        <v>160.54745997286261</v>
+      </c>
+      <c r="AM71">
+        <v>652695.16574219672</v>
+      </c>
+    </row>
+    <row r="72" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
       <c r="E72" s="10"/>
@@ -10956,8 +11151,17 @@
       <c r="Z72" s="10"/>
       <c r="AA72" s="10"/>
       <c r="AB72" s="10"/>
-    </row>
-    <row r="73" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AK72" s="9">
+        <v>3.3000000000000016</v>
+      </c>
+      <c r="AL72">
+        <v>168.22115289642232</v>
+      </c>
+      <c r="AM72">
+        <v>570980.70299198967</v>
+      </c>
+    </row>
+    <row r="73" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
       <c r="E73" s="10"/>
@@ -10989,7 +11193,7 @@
       <c r="AA73" s="10"/>
       <c r="AB73" s="10"/>
     </row>
-    <row r="74" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
       <c r="E74" s="10"/>
@@ -11020,8 +11224,9 @@
       <c r="Z74" s="10"/>
       <c r="AA74" s="10"/>
       <c r="AB74" s="10"/>
-    </row>
-    <row r="75" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AK74" s="9"/>
+    </row>
+    <row r="75" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C75" s="10"/>
       <c r="D75" s="10"/>
       <c r="E75" s="10"/>
@@ -11052,8 +11257,9 @@
       <c r="Z75" s="10"/>
       <c r="AA75" s="10"/>
       <c r="AB75" s="10"/>
-    </row>
-    <row r="76" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AK75" s="9"/>
+    </row>
+    <row r="76" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C76" s="10"/>
       <c r="D76" s="10"/>
       <c r="E76" s="10"/>
@@ -11081,7 +11287,7 @@
       <c r="AA76" s="10"/>
       <c r="AB76" s="10"/>
     </row>
-    <row r="77" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C77" s="10"/>
       <c r="D77" s="10"/>
       <c r="E77" s="10"/>
@@ -11108,20 +11314,38 @@
       <c r="Z77" s="10"/>
       <c r="AA77" s="10"/>
       <c r="AB77" s="10"/>
-    </row>
-    <row r="85" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="AK77" s="9"/>
+    </row>
+    <row r="78" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="AK78" s="9"/>
+    </row>
+    <row r="80" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="AK80" s="9"/>
+    </row>
+    <row r="81" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="AK81" s="9"/>
+    </row>
+    <row r="83" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="AK83" s="9"/>
+    </row>
+    <row r="84" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="AK84" s="9"/>
+    </row>
+    <row r="85" spans="5:37" x14ac:dyDescent="0.25">
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
     </row>
-    <row r="86" spans="5:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:37" x14ac:dyDescent="0.25">
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
-    </row>
-    <row r="87" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="AK86" s="9"/>
+    </row>
+    <row r="87" spans="5:37" x14ac:dyDescent="0.25">
       <c r="M87" s="5"/>
       <c r="N87" s="5"/>
-    </row>
-    <row r="88" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="AK87" s="9"/>
+    </row>
+    <row r="88" spans="5:37" x14ac:dyDescent="0.25">
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
@@ -11130,6 +11354,12 @@
       <c r="K88" s="1"/>
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
+    </row>
+    <row r="89" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="AK89" s="9"/>
+    </row>
+    <row r="90" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="AK90" s="9"/>
     </row>
     <row r="99" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D99" s="1"/>

</xml_diff>